<commit_message>
Full working code optimize. Unable to make my Image as main data stucture but overall it is working Todo: Test full run.
</commit_message>
<xml_diff>
--- a/output_Q2/DF_Full_Result.xlsx
+++ b/output_Q2/DF_Full_Result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="52">
   <si>
     <t>mean_fit_time</t>
   </si>
@@ -52,6 +52,9 @@
     <t>split1_test_score</t>
   </si>
   <si>
+    <t>split2_test_score</t>
+  </si>
+  <si>
     <t>mean_test_score</t>
   </si>
   <si>
@@ -61,112 +64,112 @@
     <t>rank_test_score</t>
   </si>
   <si>
+    <t>adam</t>
+  </si>
+  <si>
     <t>rmsprop</t>
   </si>
   <si>
-    <t>adam</t>
+    <t>sigmoid</t>
   </si>
   <si>
     <t>softmax</t>
   </si>
   <si>
-    <t>sigmoid</t>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
   </si>
   <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
   </si>
   <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
     <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
   </si>
   <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
   </si>
   <si>
     <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
   </si>
   <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
   </si>
   <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
   </si>
   <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
   </si>
   <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
   </si>
   <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
   </si>
   <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
   </si>
 </sst>
 </file>
@@ -524,13 +527,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,25 +579,28 @@
       <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B2">
-        <v>56.40068924427032</v>
+        <v>155.7662330468496</v>
       </c>
       <c r="C2">
-        <v>0.3234046697616577</v>
+        <v>20.28444754661299</v>
       </c>
       <c r="D2">
-        <v>5.586923003196716</v>
+        <v>5.504999717076619</v>
       </c>
       <c r="E2">
-        <v>0.0235217809677124</v>
+        <v>0.9799715240541935</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>20</v>
@@ -606,42 +612,45 @@
         <v>256</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L2">
-        <v>0.9179999828338623</v>
+        <v>0.9194029569625854</v>
       </c>
       <c r="M2">
-        <v>0.9119999408721924</v>
+        <v>0.9104477763175964</v>
       </c>
       <c r="N2">
-        <v>0.9149999618530273</v>
+        <v>0.9121212363243103</v>
       </c>
       <c r="O2">
-        <v>0.003000020980834961</v>
+        <v>0.9139906565348307</v>
       </c>
       <c r="P2">
+        <v>0.003887575425954086</v>
+      </c>
+      <c r="Q2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>2332.342237472534</v>
+        <v>139.2786092758179</v>
       </c>
       <c r="C3">
-        <v>2277.772881269455</v>
+        <v>9.527351281448826</v>
       </c>
       <c r="D3">
-        <v>5.661866068840027</v>
+        <v>4.257439215977986</v>
       </c>
       <c r="E3">
-        <v>0.2483307123184204</v>
+        <v>0.2315458659528113</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -653,95 +662,101 @@
         <v>10</v>
       </c>
       <c r="I3">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L3">
-        <v>0.9139999151229858</v>
+        <v>0.9104477763175964</v>
       </c>
       <c r="M3">
-        <v>0.9119999408721924</v>
+        <v>0.904477596282959</v>
       </c>
       <c r="N3">
-        <v>0.9129999279975891</v>
+        <v>0.9090909361839294</v>
       </c>
       <c r="O3">
-        <v>0.0009999871253967285</v>
+        <v>0.908005436261495</v>
       </c>
       <c r="P3">
+        <v>0.002555320589502078</v>
+      </c>
+      <c r="Q3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" s="1">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B4">
-        <v>70.40902101993561</v>
+        <v>136.9318378766378</v>
       </c>
       <c r="C4">
-        <v>1.700586676597595</v>
+        <v>1.274854506382764</v>
       </c>
       <c r="D4">
-        <v>7.021605968475342</v>
+        <v>4.776388168334961</v>
       </c>
       <c r="E4">
-        <v>0.1547102928161621</v>
+        <v>0.2606816074364948</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
       </c>
       <c r="G4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>10</v>
       </c>
       <c r="I4">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L4">
-        <v>0.9059999585151672</v>
+        <v>0.9134328961372375</v>
       </c>
       <c r="M4">
-        <v>0.9160000085830688</v>
+        <v>0.9044776558876038</v>
       </c>
       <c r="N4">
-        <v>0.910999983549118</v>
+        <v>0.9060605764389038</v>
       </c>
       <c r="O4">
-        <v>0.005000025033950806</v>
+        <v>0.9079903761545817</v>
       </c>
       <c r="P4">
+        <v>0.003902322145350392</v>
+      </c>
+      <c r="Q4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
-        <v>58.73139917850494</v>
+        <v>155.0160129865011</v>
       </c>
       <c r="C5">
-        <v>0.1939030885696411</v>
+        <v>8.344751594628521</v>
       </c>
       <c r="D5">
-        <v>6.011425852775574</v>
+        <v>5.827320019404094</v>
       </c>
       <c r="E5">
-        <v>0.1929837465286255</v>
+        <v>0.8863853928567742</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -756,45 +771,48 @@
         <v>256</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L5">
-        <v>0.9059999585151672</v>
+        <v>0.9164179563522339</v>
       </c>
       <c r="M5">
-        <v>0.9119999408721924</v>
+        <v>0.904477596282959</v>
       </c>
       <c r="N5">
-        <v>0.9089999496936798</v>
+        <v>0.896969735622406</v>
       </c>
       <c r="O5">
-        <v>0.002999991178512573</v>
+        <v>0.9059550960858663</v>
       </c>
       <c r="P5">
+        <v>0.008008144880462644</v>
+      </c>
+      <c r="Q5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" s="1">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>60.77713358402252</v>
+        <v>139.0637479623159</v>
       </c>
       <c r="C6">
-        <v>0.4019948244094849</v>
+        <v>11.84118828485273</v>
       </c>
       <c r="D6">
-        <v>5.93771231174469</v>
+        <v>4.541523615519206</v>
       </c>
       <c r="E6">
-        <v>0.2287987470626831</v>
+        <v>0.5061824543846188</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -806,198 +824,210 @@
         <v>256</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L6">
-        <v>0.9180000424385071</v>
+        <v>0.9164179563522339</v>
       </c>
       <c r="M6">
-        <v>0.8939999938011169</v>
+        <v>0.8985074162483215</v>
       </c>
       <c r="N6">
-        <v>0.906000018119812</v>
+        <v>0.8969696760177612</v>
       </c>
       <c r="O6">
-        <v>0.01200002431869507</v>
+        <v>0.9039650162061056</v>
       </c>
       <c r="P6">
+        <v>0.008827908395781417</v>
+      </c>
+      <c r="Q6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>61.30071353912354</v>
+        <v>53.04193234443665</v>
       </c>
       <c r="C7">
-        <v>5.363958597183228</v>
+        <v>8.771477526258465</v>
       </c>
       <c r="D7">
-        <v>5.954721093177795</v>
+        <v>5.394241571426392</v>
       </c>
       <c r="E7">
-        <v>0.1622153520584106</v>
+        <v>1.038732197673116</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I7">
         <v>256</v>
       </c>
       <c r="J7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L7">
-        <v>0.8999999761581421</v>
+        <v>0.9134328365325928</v>
       </c>
       <c r="M7">
-        <v>0.903999924659729</v>
+        <v>0.9074626564979553</v>
       </c>
       <c r="N7">
-        <v>0.9019999504089355</v>
+        <v>0.8878787755966187</v>
       </c>
       <c r="O7">
-        <v>0.001999974250793457</v>
+        <v>0.9029247562090555</v>
       </c>
       <c r="P7">
+        <v>0.01091472741616778</v>
+      </c>
+      <c r="Q7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" s="1">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <v>29.09433197975159</v>
+        <v>133.3880138397217</v>
       </c>
       <c r="C8">
-        <v>0.9804730415344238</v>
+        <v>2.622285475432505</v>
       </c>
       <c r="D8">
-        <v>5.69726574420929</v>
+        <v>5.162713925043742</v>
       </c>
       <c r="E8">
-        <v>0.08128297328948975</v>
+        <v>0.2269020638316955</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8">
         <v>20</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I8">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L8">
-        <v>0.8960000872612</v>
+        <v>0.9074625968933105</v>
       </c>
       <c r="M8">
-        <v>0.9059999585151672</v>
+        <v>0.8895522356033325</v>
       </c>
       <c r="N8">
-        <v>0.9010000228881836</v>
+        <v>0.9060605764389038</v>
       </c>
       <c r="O8">
-        <v>0.004999935626983643</v>
+        <v>0.901025136311849</v>
       </c>
       <c r="P8">
+        <v>0.008132732355088356</v>
+      </c>
+      <c r="Q8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" s="1">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9">
-        <v>29.37954354286194</v>
+        <v>140.4387857913971</v>
       </c>
       <c r="C9">
-        <v>0.6546580791473389</v>
+        <v>2.884168499334205</v>
       </c>
       <c r="D9">
-        <v>5.637627601623535</v>
+        <v>5.040391445159912</v>
       </c>
       <c r="E9">
-        <v>0.08248162269592285</v>
+        <v>0.4871967504003464</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
       </c>
       <c r="G9">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I9">
         <v>128</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L9">
-        <v>0.8919999599456787</v>
+        <v>0.8955223560333252</v>
       </c>
       <c r="M9">
-        <v>0.9100000262260437</v>
+        <v>0.9074626564979553</v>
       </c>
       <c r="N9">
-        <v>0.9009999930858612</v>
+        <v>0.8939393758773804</v>
       </c>
       <c r="O9">
-        <v>0.009000033140182495</v>
+        <v>0.8989747961362203</v>
       </c>
       <c r="P9">
+        <v>0.006036515920283998</v>
+      </c>
+      <c r="Q9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B10">
-        <v>54.73745203018188</v>
+        <v>146.0741839408875</v>
       </c>
       <c r="C10">
-        <v>0.336683988571167</v>
+        <v>4.042508879079694</v>
       </c>
       <c r="D10">
-        <v>5.394711017608643</v>
+        <v>15.03789019584656</v>
       </c>
       <c r="E10">
-        <v>0.01310133934020996</v>
+        <v>6.291689010555989</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G10">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H10">
         <v>10</v>
@@ -1006,198 +1036,210 @@
         <v>128</v>
       </c>
       <c r="J10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10">
+        <v>0.9134328365325928</v>
+      </c>
+      <c r="M10">
+        <v>0.89552241563797</v>
+      </c>
+      <c r="N10">
+        <v>0.8878788352012634</v>
+      </c>
+      <c r="O10">
+        <v>0.8989446957906088</v>
+      </c>
+      <c r="P10">
+        <v>0.01070936497005477</v>
+      </c>
+      <c r="Q10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>733.694678068161</v>
+      </c>
+      <c r="C11">
+        <v>879.9061287312825</v>
+      </c>
+      <c r="D11">
+        <v>5.900887330373128</v>
+      </c>
+      <c r="E11">
+        <v>2.327244264434575</v>
+      </c>
+      <c r="F11" t="s">
         <v>17</v>
       </c>
-      <c r="K10" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10">
-        <v>0.8859999775886536</v>
-      </c>
-      <c r="M10">
-        <v>0.9140000939369202</v>
-      </c>
-      <c r="N10">
-        <v>0.9000000357627869</v>
-      </c>
-      <c r="O10">
-        <v>0.0140000581741333</v>
-      </c>
-      <c r="P10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="1">
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>128</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11">
+        <v>0.9253730773925781</v>
+      </c>
+      <c r="M11">
+        <v>0.8985075354576111</v>
+      </c>
+      <c r="N11">
+        <v>0.8696969747543335</v>
+      </c>
+      <c r="O11">
+        <v>0.8978591958681742</v>
+      </c>
+      <c r="P11">
+        <v>0.02273429654968474</v>
+      </c>
+      <c r="Q11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="1">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>74.07484992345174</v>
+      </c>
+      <c r="C12">
+        <v>20.03521622423804</v>
+      </c>
+      <c r="D12">
+        <v>5.643171469370524</v>
+      </c>
+      <c r="E12">
+        <v>1.091181337797907</v>
+      </c>
+      <c r="F12" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <v>35.03264975547791</v>
-      </c>
-      <c r="C11">
-        <v>0.4320721626281738</v>
-      </c>
-      <c r="D11">
-        <v>7.118086576461792</v>
-      </c>
-      <c r="E11">
-        <v>0.02605104446411133</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11">
-        <v>25</v>
-      </c>
-      <c r="H11">
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
         <v>5</v>
-      </c>
-      <c r="I11">
-        <v>256</v>
-      </c>
-      <c r="J11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11">
-        <v>0.8899999856948853</v>
-      </c>
-      <c r="M11">
-        <v>0.9099998474121094</v>
-      </c>
-      <c r="N11">
-        <v>0.8999999165534973</v>
-      </c>
-      <c r="O11">
-        <v>0.009999930858612061</v>
-      </c>
-      <c r="P11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>53.94450795650482</v>
-      </c>
-      <c r="C12">
-        <v>0.1488054990768433</v>
-      </c>
-      <c r="D12">
-        <v>5.411806464195251</v>
-      </c>
-      <c r="E12">
-        <v>0.07452285289764404</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12">
-        <v>25</v>
-      </c>
-      <c r="H12">
-        <v>10</v>
       </c>
       <c r="I12">
         <v>256</v>
       </c>
       <c r="J12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12">
+        <v>0.8955223560333252</v>
+      </c>
+      <c r="M12">
+        <v>0.9134328365325928</v>
+      </c>
+      <c r="N12">
+        <v>0.8696969151496887</v>
+      </c>
+      <c r="O12">
+        <v>0.8928840359052023</v>
+      </c>
+      <c r="P12">
+        <v>0.01795231191475042</v>
+      </c>
+      <c r="Q12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>125.287312189738</v>
+      </c>
+      <c r="C13">
+        <v>2.848083827545802</v>
+      </c>
+      <c r="D13">
+        <v>5.21040137608846</v>
+      </c>
+      <c r="E13">
+        <v>0.3132591712494442</v>
+      </c>
+      <c r="F13" t="s">
         <v>17</v>
       </c>
-      <c r="K12" t="s">
-        <v>29</v>
-      </c>
-      <c r="L12">
-        <v>0.8979999423027039</v>
-      </c>
-      <c r="M12">
-        <v>0.8980000019073486</v>
-      </c>
-      <c r="N12">
-        <v>0.8979999721050262</v>
-      </c>
-      <c r="O12">
-        <v>2.980232238769531e-08</v>
-      </c>
-      <c r="P12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="1">
-        <v>23</v>
-      </c>
-      <c r="B13">
-        <v>55.45402669906616</v>
-      </c>
-      <c r="C13">
-        <v>1.225035905838013</v>
-      </c>
-      <c r="D13">
-        <v>5.378617167472839</v>
-      </c>
-      <c r="E13">
-        <v>0.06781876087188721</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
       <c r="G13">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J13" t="s">
         <v>18</v>
       </c>
       <c r="K13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L13">
-        <v>0.8939999938011169</v>
+        <v>0.9194030165672302</v>
       </c>
       <c r="M13">
-        <v>0.9019999504089355</v>
+        <v>0.9014924764633179</v>
       </c>
       <c r="N13">
-        <v>0.8979999721050262</v>
+        <v>0.8515151143074036</v>
       </c>
       <c r="O13">
-        <v>0.003999978303909302</v>
+        <v>0.8908035357793173</v>
       </c>
       <c r="P13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>0.02872724500098014</v>
+      </c>
+      <c r="Q13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="1">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B14">
-        <v>69.07200527191162</v>
+        <v>130.9250098864237</v>
       </c>
       <c r="C14">
-        <v>0.2381596565246582</v>
+        <v>2.928556346320716</v>
       </c>
       <c r="D14">
-        <v>7.246112465858459</v>
+        <v>4.804123481114705</v>
       </c>
       <c r="E14">
-        <v>0.07331502437591553</v>
+        <v>0.216546873076932</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
       </c>
       <c r="G14">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H14">
         <v>10</v>
@@ -1206,92 +1248,98 @@
         <v>128</v>
       </c>
       <c r="J14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L14">
-        <v>0.8819999694824219</v>
+        <v>0.8895522952079773</v>
       </c>
       <c r="M14">
-        <v>0.9119999408721924</v>
+        <v>0.8746268153190613</v>
       </c>
       <c r="N14">
-        <v>0.8969999551773071</v>
+        <v>0.9060606360435486</v>
       </c>
       <c r="O14">
-        <v>0.01499998569488525</v>
+        <v>0.8900799155235291</v>
       </c>
       <c r="P14">
+        <v>0.01283822570121066</v>
+      </c>
+      <c r="Q14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="A15" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>29.59978711605072</v>
+        <v>66.49570528666179</v>
       </c>
       <c r="C15">
-        <v>0.4164911508560181</v>
+        <v>12.04353351159397</v>
       </c>
       <c r="D15">
-        <v>5.784807562828064</v>
+        <v>8.22185722986857</v>
       </c>
       <c r="E15">
-        <v>0.05113875865936279</v>
+        <v>4.701438716648958</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
       </c>
       <c r="G15">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H15">
         <v>5</v>
       </c>
       <c r="I15">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J15" t="s">
         <v>18</v>
       </c>
       <c r="K15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L15">
-        <v>0.8899999856948853</v>
+        <v>0.8985074758529663</v>
       </c>
       <c r="M15">
-        <v>0.9020000696182251</v>
+        <v>0.8865671753883362</v>
       </c>
       <c r="N15">
-        <v>0.8960000276565552</v>
+        <v>0.8787878751754761</v>
       </c>
       <c r="O15">
-        <v>0.006000041961669922</v>
+        <v>0.8879541754722595</v>
       </c>
       <c r="P15">
+        <v>0.008110013959894309</v>
+      </c>
+      <c r="Q15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17">
       <c r="A16" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B16">
-        <v>58.18089687824249</v>
+        <v>74.36285765965779</v>
       </c>
       <c r="C16">
-        <v>1.342935919761658</v>
+        <v>14.00122835394506</v>
       </c>
       <c r="D16">
-        <v>6.294667363166809</v>
+        <v>11.3113473256429</v>
       </c>
       <c r="E16">
-        <v>0.3016945123672485</v>
+        <v>6.680864780809817</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
@@ -1300,104 +1348,110 @@
         <v>20</v>
       </c>
       <c r="H16">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I16">
         <v>128</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L16">
-        <v>0.8839999437332153</v>
+        <v>0.9074625968933105</v>
       </c>
       <c r="M16">
-        <v>0.9000000953674316</v>
+        <v>0.8716417551040649</v>
       </c>
       <c r="N16">
-        <v>0.8920000195503235</v>
+        <v>0.8787878751754761</v>
       </c>
       <c r="O16">
-        <v>0.008000075817108154</v>
+        <v>0.8859640757242838</v>
       </c>
       <c r="P16">
+        <v>0.01547915948105867</v>
+      </c>
+      <c r="Q16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17">
       <c r="A17" s="1">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>74.33030064900716</v>
+      </c>
+      <c r="C17">
+        <v>17.05531198814253</v>
+      </c>
+      <c r="D17">
+        <v>5.555164575576782</v>
+      </c>
+      <c r="E17">
+        <v>1.672171763965501</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>20</v>
+      </c>
+      <c r="H17">
         <v>5</v>
-      </c>
-      <c r="B17">
-        <v>54.39064157009125</v>
-      </c>
-      <c r="C17">
-        <v>0.009059548377990723</v>
-      </c>
-      <c r="D17">
-        <v>5.498298168182373</v>
-      </c>
-      <c r="E17">
-        <v>0.04487967491149902</v>
-      </c>
-      <c r="F17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17">
-        <v>25</v>
-      </c>
-      <c r="H17">
-        <v>10</v>
       </c>
       <c r="I17">
         <v>256</v>
       </c>
       <c r="J17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L17">
-        <v>0.871999979019165</v>
+        <v>0.886567234992981</v>
       </c>
       <c r="M17">
-        <v>0.9040000438690186</v>
+        <v>0.8776119947433472</v>
       </c>
       <c r="N17">
-        <v>0.8880000114440918</v>
+        <v>0.8757575154304504</v>
       </c>
       <c r="O17">
-        <v>0.01600003242492676</v>
+        <v>0.8799789150555929</v>
       </c>
       <c r="P17">
+        <v>0.004719762923320736</v>
+      </c>
+      <c r="Q17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17">
       <c r="A18" s="1">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B18">
-        <v>34.67000830173492</v>
+        <v>66.62978466351827</v>
       </c>
       <c r="C18">
-        <v>0.1661816835403442</v>
+        <v>17.38780785568654</v>
       </c>
       <c r="D18">
-        <v>7.090117454528809</v>
+        <v>8.318903843561808</v>
       </c>
       <c r="E18">
-        <v>0.2034189701080322</v>
+        <v>4.423451633198773</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
       </c>
       <c r="G18">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -1406,45 +1460,48 @@
         <v>128</v>
       </c>
       <c r="J18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" t="s">
+        <v>36</v>
+      </c>
+      <c r="L18">
+        <v>0.8686566948890686</v>
+      </c>
+      <c r="M18">
+        <v>0.8746268749237061</v>
+      </c>
+      <c r="N18">
+        <v>0.8939393162727356</v>
+      </c>
+      <c r="O18">
+        <v>0.8790742953618368</v>
+      </c>
+      <c r="P18">
+        <v>0.01079003853631027</v>
+      </c>
+      <c r="Q18">
         <v>17</v>
       </c>
-      <c r="K18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18">
-        <v>0.8779999613761902</v>
-      </c>
-      <c r="M18">
-        <v>0.8980000019073486</v>
-      </c>
-      <c r="N18">
-        <v>0.8879999816417694</v>
-      </c>
-      <c r="O18">
-        <v>0.01000002026557922</v>
-      </c>
-      <c r="P18">
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="1">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>115.3827340602875</v>
+      </c>
+      <c r="C19">
+        <v>2.938009680901168</v>
+      </c>
+      <c r="D19">
+        <v>10.52469603220622</v>
+      </c>
+      <c r="E19">
+        <v>3.925206061234818</v>
+      </c>
+      <c r="F19" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="1">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>70.5338716506958</v>
-      </c>
-      <c r="C19">
-        <v>0.8459038734436035</v>
-      </c>
-      <c r="D19">
-        <v>7.076645374298096</v>
-      </c>
-      <c r="E19">
-        <v>0.07676863670349121</v>
-      </c>
-      <c r="F19" t="s">
-        <v>16</v>
       </c>
       <c r="G19">
         <v>25</v>
@@ -1456,98 +1513,104 @@
         <v>256</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L19">
-        <v>0.8900001049041748</v>
+        <v>0.8029851317405701</v>
       </c>
       <c r="M19">
-        <v>0.8840000033378601</v>
+        <v>0.904477596282959</v>
       </c>
       <c r="N19">
-        <v>0.8870000541210175</v>
+        <v>0.9060606360435486</v>
       </c>
       <c r="O19">
-        <v>0.003000050783157349</v>
+        <v>0.8711744546890259</v>
       </c>
       <c r="P19">
+        <v>0.04822146359487307</v>
+      </c>
+      <c r="Q19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17">
       <c r="A20" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>69.28030145168304</v>
+        <v>131.4374632835388</v>
       </c>
       <c r="C20">
-        <v>0.7380827665328979</v>
+        <v>3.014324335015929</v>
       </c>
       <c r="D20">
-        <v>6.938002109527588</v>
+        <v>9.672802925109863</v>
       </c>
       <c r="E20">
-        <v>0.06128191947937012</v>
+        <v>6.497336663406538</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G20">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L20">
-        <v>0.8759999871253967</v>
+        <v>0.8686566948890686</v>
       </c>
       <c r="M20">
-        <v>0.8939999938011169</v>
+        <v>0.8507463335990906</v>
       </c>
       <c r="N20">
-        <v>0.8849999904632568</v>
+        <v>0.8939393758773804</v>
       </c>
       <c r="O20">
-        <v>0.009000003337860107</v>
+        <v>0.8711141347885132</v>
       </c>
       <c r="P20">
+        <v>0.01771889732193794</v>
+      </c>
+      <c r="Q20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="A21" s="1">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>66.64421427249908</v>
+        <v>112.6923964818319</v>
       </c>
       <c r="C21">
-        <v>3.541003823280334</v>
+        <v>4.399059745862806</v>
       </c>
       <c r="D21">
-        <v>6.86751663684845</v>
+        <v>4.189464012781779</v>
       </c>
       <c r="E21">
-        <v>0.1956886053085327</v>
+        <v>0.3503958701721298</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G21">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H21">
         <v>10</v>
@@ -1556,48 +1619,51 @@
         <v>128</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L21">
-        <v>0.8959999680519104</v>
+        <v>0.8656716346740723</v>
       </c>
       <c r="M21">
-        <v>0.871999979019165</v>
+        <v>0.8716418147087097</v>
       </c>
       <c r="N21">
-        <v>0.8839999735355377</v>
+        <v>0.8696969747543335</v>
       </c>
       <c r="O21">
-        <v>0.01199999451637268</v>
+        <v>0.8690034747123718</v>
       </c>
       <c r="P21">
+        <v>0.002486157563074196</v>
+      </c>
+      <c r="Q21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="A22" s="1">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B22">
-        <v>28.00593602657318</v>
+        <v>64.02316840489705</v>
       </c>
       <c r="C22">
-        <v>0.2026373147964478</v>
+        <v>15.66647370593406</v>
       </c>
       <c r="D22">
-        <v>5.515504240989685</v>
+        <v>9.666007916132608</v>
       </c>
       <c r="E22">
-        <v>0.02817738056182861</v>
+        <v>6.74894285778613</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G22">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H22">
         <v>5</v>
@@ -1606,101 +1672,107 @@
         <v>128</v>
       </c>
       <c r="J22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22">
+        <v>0.8417910933494568</v>
+      </c>
+      <c r="M22">
+        <v>0.8805969953536987</v>
+      </c>
+      <c r="N22">
+        <v>0.8818181753158569</v>
+      </c>
+      <c r="O22">
+        <v>0.8680687546730042</v>
+      </c>
+      <c r="P22">
+        <v>0.01858779946813298</v>
+      </c>
+      <c r="Q22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="1">
         <v>17</v>
       </c>
-      <c r="K22" t="s">
-        <v>39</v>
-      </c>
-      <c r="L22">
-        <v>0.8999999165534973</v>
-      </c>
-      <c r="M22">
-        <v>0.8619999885559082</v>
-      </c>
-      <c r="N22">
-        <v>0.8809999525547028</v>
-      </c>
-      <c r="O22">
-        <v>0.01899996399879456</v>
-      </c>
-      <c r="P22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="1">
-        <v>27</v>
-      </c>
       <c r="B23">
-        <v>30.49364125728607</v>
+        <v>65.43442940711975</v>
       </c>
       <c r="C23">
-        <v>1.677332997322083</v>
+        <v>15.62040132981878</v>
       </c>
       <c r="D23">
-        <v>6.008776903152466</v>
+        <v>5.197110017140706</v>
       </c>
       <c r="E23">
-        <v>0.3219826221466064</v>
+        <v>1.205024106710354</v>
       </c>
       <c r="F23" t="s">
         <v>16</v>
       </c>
       <c r="G23">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H23">
         <v>5</v>
       </c>
       <c r="I23">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J23" t="s">
         <v>18</v>
       </c>
       <c r="K23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L23">
-        <v>0.8660000562667847</v>
+        <v>0.8298507332801819</v>
       </c>
       <c r="M23">
-        <v>0.8799999952316284</v>
+        <v>0.880596935749054</v>
       </c>
       <c r="N23">
-        <v>0.8730000257492065</v>
+        <v>0.8818182349205017</v>
       </c>
       <c r="O23">
-        <v>0.006999969482421875</v>
+        <v>0.8640886346499125</v>
       </c>
       <c r="P23">
+        <v>0.02421498586370427</v>
+      </c>
+      <c r="Q23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="A24" s="1">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B24">
-        <v>35.58597874641418</v>
+        <v>992.8292651176453</v>
       </c>
       <c r="C24">
-        <v>0.1367595195770264</v>
+        <v>1245.974226839766</v>
       </c>
       <c r="D24">
-        <v>7.082001090049744</v>
+        <v>4.191378911336263</v>
       </c>
       <c r="E24">
-        <v>0.05192291736602783</v>
+        <v>0.1403756232513582</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G24">
         <v>25</v>
       </c>
       <c r="H24">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I24">
         <v>128</v>
@@ -1709,195 +1781,207 @@
         <v>18</v>
       </c>
       <c r="K24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L24">
-        <v>0.8560000061988831</v>
+        <v>0.8716418147087097</v>
       </c>
       <c r="M24">
-        <v>0.8840000033378601</v>
+        <v>0.89552241563797</v>
       </c>
       <c r="N24">
-        <v>0.8700000047683716</v>
+        <v>0.8242424726486206</v>
       </c>
       <c r="O24">
-        <v>0.01399999856948853</v>
+        <v>0.8638022343317667</v>
       </c>
       <c r="P24">
+        <v>0.02962320974625736</v>
+      </c>
+      <c r="Q24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17">
       <c r="A25" s="1">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>60.55417084693909</v>
+      </c>
+      <c r="C25">
+        <v>12.28426764377543</v>
+      </c>
+      <c r="D25">
+        <v>5.947096586227417</v>
+      </c>
+      <c r="E25">
+        <v>1.567065480771697</v>
+      </c>
+      <c r="F25" t="s">
         <v>17</v>
       </c>
-      <c r="B25">
-        <v>35.04812800884247</v>
-      </c>
-      <c r="C25">
-        <v>0.1133395433425903</v>
-      </c>
-      <c r="D25">
-        <v>6.909010171890259</v>
-      </c>
-      <c r="E25">
-        <v>0.02202796936035156</v>
-      </c>
-      <c r="F25" t="s">
-        <v>16</v>
-      </c>
       <c r="G25">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H25">
         <v>5</v>
       </c>
       <c r="I25">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L25">
-        <v>0.8579999804496765</v>
+        <v>0.8776119351387024</v>
       </c>
       <c r="M25">
-        <v>0.8779999613761902</v>
+        <v>0.8238806128501892</v>
       </c>
       <c r="N25">
-        <v>0.8679999709129333</v>
+        <v>0.8878788352012634</v>
       </c>
       <c r="O25">
-        <v>0.009999990463256836</v>
+        <v>0.8631237943967184</v>
       </c>
       <c r="P25">
+        <v>0.02806388880921575</v>
+      </c>
+      <c r="Q25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:17">
       <c r="A26" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B26">
-        <v>28.25281715393066</v>
+        <v>56.7287171681722</v>
       </c>
       <c r="C26">
-        <v>0.3603494167327881</v>
+        <v>9.540145426381693</v>
       </c>
       <c r="D26">
-        <v>5.620472073554993</v>
+        <v>6.073423385620117</v>
       </c>
       <c r="E26">
-        <v>0.1610685586929321</v>
+        <v>3.233729008795648</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G26">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H26">
         <v>5</v>
       </c>
       <c r="I26">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J26" t="s">
         <v>18</v>
       </c>
       <c r="K26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L26">
-        <v>0.8520001173019409</v>
+        <v>0.8985074162483215</v>
       </c>
       <c r="M26">
-        <v>0.8820000290870667</v>
+        <v>0.8059701323509216</v>
       </c>
       <c r="N26">
-        <v>0.8670000731945038</v>
+        <v>0.8787878751754761</v>
       </c>
       <c r="O26">
-        <v>0.01499995589256287</v>
+        <v>0.8610884745915731</v>
       </c>
       <c r="P26">
+        <v>0.03979730990531141</v>
+      </c>
+      <c r="Q26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17">
       <c r="A27" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B27">
-        <v>55.04668033123016</v>
+        <v>46.43642870585123</v>
       </c>
       <c r="C27">
-        <v>0.5830978155136108</v>
+        <v>7.561643605093507</v>
       </c>
       <c r="D27">
-        <v>5.643908262252808</v>
+        <v>5.112329403559367</v>
       </c>
       <c r="E27">
-        <v>0.09773778915405273</v>
+        <v>1.254999875879873</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G27">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H27">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I27">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J27" t="s">
         <v>18</v>
       </c>
       <c r="K27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L27">
-        <v>0.8199999928474426</v>
+        <v>0.8537313342094421</v>
       </c>
       <c r="M27">
-        <v>0.8980000019073486</v>
+        <v>0.8776119351387024</v>
       </c>
       <c r="N27">
-        <v>0.8589999973773956</v>
+        <v>0.8484849333763123</v>
       </c>
       <c r="O27">
-        <v>0.039000004529953</v>
+        <v>0.8599427342414856</v>
       </c>
       <c r="P27">
+        <v>0.01267626852784687</v>
+      </c>
+      <c r="Q27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17">
       <c r="A28" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B28">
-        <v>26.89967262744904</v>
+        <v>68.62597346305847</v>
       </c>
       <c r="C28">
-        <v>0.2045830488204956</v>
+        <v>13.95137037377635</v>
       </c>
       <c r="D28">
-        <v>5.420054912567139</v>
+        <v>7.028938372929891</v>
       </c>
       <c r="E28">
-        <v>0.1720874309539795</v>
+        <v>3.453449339573602</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G28">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H28">
         <v>5</v>
@@ -1909,42 +1993,45 @@
         <v>18</v>
       </c>
       <c r="K28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L28">
-        <v>0.8439999222755432</v>
+        <v>0.8298507928848267</v>
       </c>
       <c r="M28">
-        <v>0.8659999966621399</v>
+        <v>0.8626866340637207</v>
       </c>
       <c r="N28">
-        <v>0.8549999594688416</v>
+        <v>0.8818181753158569</v>
       </c>
       <c r="O28">
-        <v>0.01100003719329834</v>
+        <v>0.8581185340881348</v>
       </c>
       <c r="P28">
+        <v>0.02146008484331551</v>
+      </c>
+      <c r="Q28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17">
       <c r="A29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29">
-        <v>28.97624504566193</v>
+        <v>49.26799861590067</v>
       </c>
       <c r="C29">
-        <v>0.8505622148513794</v>
+        <v>12.35363734708296</v>
       </c>
       <c r="D29">
-        <v>6.523600339889526</v>
+        <v>5.058491468429565</v>
       </c>
       <c r="E29">
-        <v>0.3271510601043701</v>
+        <v>1.325063356764046</v>
       </c>
       <c r="F29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G29">
         <v>25</v>
@@ -1956,95 +2043,101 @@
         <v>256</v>
       </c>
       <c r="J29" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L29">
-        <v>0.8379999399185181</v>
+        <v>0.9164179563522339</v>
       </c>
       <c r="M29">
-        <v>0.8659999966621399</v>
+        <v>0.8029851317405701</v>
       </c>
       <c r="N29">
-        <v>0.851999968290329</v>
+        <v>0.8030303120613098</v>
       </c>
       <c r="O29">
-        <v>0.01400002837181091</v>
+        <v>0.8408111333847046</v>
       </c>
       <c r="P29">
+        <v>0.05346210040609972</v>
+      </c>
+      <c r="Q29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17">
       <c r="A30" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B30">
-        <v>26.96062707901001</v>
+        <v>113.65762702624</v>
       </c>
       <c r="C30">
-        <v>0.8500068187713623</v>
+        <v>0.8220505812669434</v>
       </c>
       <c r="D30">
-        <v>5.57010543346405</v>
+        <v>3.905224720637003</v>
       </c>
       <c r="E30">
-        <v>0.02692806720733643</v>
+        <v>0.01385025860172755</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G30">
         <v>25</v>
       </c>
       <c r="H30">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I30">
         <v>256</v>
       </c>
       <c r="J30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" t="s">
+        <v>48</v>
+      </c>
+      <c r="L30">
+        <v>0.9074627161026001</v>
+      </c>
+      <c r="M30">
+        <v>0.6955223679542542</v>
+      </c>
+      <c r="N30">
+        <v>0.8393939733505249</v>
+      </c>
+      <c r="O30">
+        <v>0.8141263524691263</v>
+      </c>
+      <c r="P30">
+        <v>0.08834974926229308</v>
+      </c>
+      <c r="Q30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="1">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>39.81176551183065</v>
+      </c>
+      <c r="C31">
+        <v>0.4984907894750415</v>
+      </c>
+      <c r="D31">
+        <v>4.125336011250814</v>
+      </c>
+      <c r="E31">
+        <v>0.1356334921386906</v>
+      </c>
+      <c r="F31" t="s">
         <v>17</v>
-      </c>
-      <c r="K30" t="s">
-        <v>47</v>
-      </c>
-      <c r="L30">
-        <v>0.8259999752044678</v>
-      </c>
-      <c r="M30">
-        <v>0.8519999980926514</v>
-      </c>
-      <c r="N30">
-        <v>0.8389999866485596</v>
-      </c>
-      <c r="O30">
-        <v>0.0130000114440918</v>
-      </c>
-      <c r="P30">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="1">
-        <v>9</v>
-      </c>
-      <c r="B31">
-        <v>28.25944554805756</v>
-      </c>
-      <c r="C31">
-        <v>0.2363790273666382</v>
-      </c>
-      <c r="D31">
-        <v>5.554647326469421</v>
-      </c>
-      <c r="E31">
-        <v>0.05834376811981201</v>
-      </c>
-      <c r="F31" t="s">
-        <v>15</v>
       </c>
       <c r="G31">
         <v>20</v>
@@ -2056,45 +2149,48 @@
         <v>256</v>
       </c>
       <c r="J31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K31" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L31">
-        <v>0.8100000023841858</v>
+        <v>0.832835853099823</v>
       </c>
       <c r="M31">
-        <v>0.8659999966621399</v>
+        <v>0.8208954930305481</v>
       </c>
       <c r="N31">
-        <v>0.8379999995231628</v>
+        <v>0.7666667103767395</v>
       </c>
       <c r="O31">
-        <v>0.02799999713897705</v>
+        <v>0.8067993521690369</v>
       </c>
       <c r="P31">
+        <v>0.02879368857426483</v>
+      </c>
+      <c r="Q31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:17">
       <c r="A32" s="1">
         <v>2</v>
       </c>
       <c r="B32">
-        <v>26.67560243606567</v>
+        <v>61.74911745389303</v>
       </c>
       <c r="C32">
-        <v>0.3544564247131348</v>
+        <v>15.04025513510453</v>
       </c>
       <c r="D32">
-        <v>5.230021357536316</v>
+        <v>5.119652668635051</v>
       </c>
       <c r="E32">
-        <v>0.01097643375396729</v>
+        <v>1.152323703920358</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G32">
         <v>25</v>
@@ -2106,74 +2202,80 @@
         <v>128</v>
       </c>
       <c r="J32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K32" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32">
+        <v>0.8298507332801819</v>
+      </c>
+      <c r="M32">
+        <v>0.7970149517059326</v>
+      </c>
+      <c r="N32">
+        <v>0.7848484516143799</v>
+      </c>
+      <c r="O32">
+        <v>0.8039047122001648</v>
+      </c>
+      <c r="P32">
+        <v>0.01900706778250232</v>
+      </c>
+      <c r="Q32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" s="1">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>57.46216837565104</v>
+      </c>
+      <c r="C33">
+        <v>11.97215545140205</v>
+      </c>
+      <c r="D33">
+        <v>9.077148278554281</v>
+      </c>
+      <c r="E33">
+        <v>6.496483655854372</v>
+      </c>
+      <c r="F33" t="s">
         <v>17</v>
       </c>
-      <c r="K32" t="s">
-        <v>49</v>
-      </c>
-      <c r="L32">
-        <v>0.8679999709129333</v>
-      </c>
-      <c r="M32">
-        <v>0.7799999713897705</v>
-      </c>
-      <c r="N32">
-        <v>0.8239999711513519</v>
-      </c>
-      <c r="O32">
-        <v>0.04399999976158142</v>
-      </c>
-      <c r="P32">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="1">
-        <v>8</v>
-      </c>
-      <c r="B33">
-        <v>27.96439218521118</v>
-      </c>
-      <c r="C33">
-        <v>0.198300838470459</v>
-      </c>
-      <c r="D33">
-        <v>5.609001755714417</v>
-      </c>
-      <c r="E33">
-        <v>0.01994597911834717</v>
-      </c>
-      <c r="F33" t="s">
-        <v>15</v>
-      </c>
       <c r="G33">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H33">
         <v>5</v>
       </c>
       <c r="I33">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L33">
-        <v>0.7820000648498535</v>
+        <v>0.8059701323509216</v>
       </c>
       <c r="M33">
-        <v>0.8199999928474426</v>
+        <v>0.8059701323509216</v>
       </c>
       <c r="N33">
-        <v>0.8010000288486481</v>
+        <v>0.7878788113594055</v>
       </c>
       <c r="O33">
-        <v>0.01899996399879456</v>
+        <v>0.7999396920204163</v>
       </c>
       <c r="P33">
+        <v>0.008528330502482386</v>
+      </c>
+      <c r="Q33">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All code and documentation done
</commit_message>
<xml_diff>
--- a/output_Q2/DF_Full_Result.xlsx
+++ b/output_Q2/DF_Full_Result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="51">
   <si>
     <t>mean_fit_time</t>
   </si>
@@ -52,9 +52,6 @@
     <t>split1_test_score</t>
   </si>
   <si>
-    <t>split2_test_score</t>
-  </si>
-  <si>
     <t>mean_test_score</t>
   </si>
   <si>
@@ -64,112 +61,112 @@
     <t>rank_test_score</t>
   </si>
   <si>
+    <t>rmsprop</t>
+  </si>
+  <si>
     <t>adam</t>
   </si>
   <si>
-    <t>rmsprop</t>
-  </si>
-  <si>
     <t>sigmoid</t>
   </si>
   <si>
     <t>softmax</t>
   </si>
   <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
     <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
   </si>
   <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
   </si>
   <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
   </si>
   <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
   </si>
   <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
   </si>
   <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
   </si>
 </sst>
 </file>
@@ -527,13 +524,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,31 +576,28 @@
       <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="1">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>112.3461164236069</v>
+      </c>
+      <c r="C2">
+        <v>1.52138888835907</v>
+      </c>
+      <c r="D2">
+        <v>10.59885251522064</v>
+      </c>
+      <c r="E2">
+        <v>0.3773878812789917</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="1">
-        <v>29</v>
-      </c>
-      <c r="B2">
-        <v>155.7662330468496</v>
-      </c>
-      <c r="C2">
-        <v>20.28444754661299</v>
-      </c>
-      <c r="D2">
-        <v>5.504999717076619</v>
-      </c>
-      <c r="E2">
-        <v>0.9799715240541935</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
       <c r="G2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -612,45 +606,42 @@
         <v>256</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2">
-        <v>0.9194029569625854</v>
+        <v>0.9359999895095825</v>
       </c>
       <c r="M2">
-        <v>0.9104477763175964</v>
+        <v>0.9320000410079956</v>
       </c>
       <c r="N2">
-        <v>0.9121212363243103</v>
+        <v>0.9340000152587891</v>
       </c>
       <c r="O2">
-        <v>0.9139906565348307</v>
+        <v>0.001999974250793457</v>
       </c>
       <c r="P2">
-        <v>0.003887575425954086</v>
-      </c>
-      <c r="Q2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:16">
       <c r="A3" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3">
-        <v>139.2786092758179</v>
+        <v>138.8890740871429</v>
       </c>
       <c r="C3">
-        <v>9.527351281448826</v>
+        <v>6.420517921447754</v>
       </c>
       <c r="D3">
-        <v>4.257439215977986</v>
+        <v>14.20784938335419</v>
       </c>
       <c r="E3">
-        <v>0.2315458659528113</v>
+        <v>1.375924229621887</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -662,101 +653,95 @@
         <v>10</v>
       </c>
       <c r="I3">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>0.9309999942779541</v>
+      </c>
+      <c r="M3">
+        <v>0.9300000071525574</v>
+      </c>
+      <c r="N3">
+        <v>0.9305000007152557</v>
+      </c>
+      <c r="O3">
+        <v>0.0004999935626983643</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="1">
         <v>21</v>
       </c>
-      <c r="L3">
-        <v>0.9104477763175964</v>
-      </c>
-      <c r="M3">
-        <v>0.904477596282959</v>
-      </c>
-      <c r="N3">
-        <v>0.9090909361839294</v>
-      </c>
-      <c r="O3">
-        <v>0.908005436261495</v>
-      </c>
-      <c r="P3">
-        <v>0.002555320589502078</v>
-      </c>
-      <c r="Q3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="1">
-        <v>30</v>
-      </c>
       <c r="B4">
-        <v>136.9318378766378</v>
+        <v>165.5413037538528</v>
       </c>
       <c r="C4">
-        <v>1.274854506382764</v>
+        <v>19.59417903423309</v>
       </c>
       <c r="D4">
-        <v>4.776388168334961</v>
+        <v>30.81350088119507</v>
       </c>
       <c r="E4">
-        <v>0.2606816074364948</v>
+        <v>16.31952834129333</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H4">
         <v>10</v>
       </c>
       <c r="I4">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L4">
-        <v>0.9134328961372375</v>
+        <v>0.9300000071525574</v>
       </c>
       <c r="M4">
-        <v>0.9044776558876038</v>
+        <v>0.9309999942779541</v>
       </c>
       <c r="N4">
-        <v>0.9060605764389038</v>
+        <v>0.9305000007152557</v>
       </c>
       <c r="O4">
-        <v>0.9079903761545817</v>
+        <v>0.0004999935626983643</v>
       </c>
       <c r="P4">
-        <v>0.003902322145350392</v>
-      </c>
-      <c r="Q4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B5">
-        <v>155.0160129865011</v>
+        <v>147.7576627731323</v>
       </c>
       <c r="C5">
-        <v>8.344751594628521</v>
+        <v>0.3653357028961182</v>
       </c>
       <c r="D5">
-        <v>5.827320019404094</v>
+        <v>16.03926026821136</v>
       </c>
       <c r="E5">
-        <v>0.8863853928567742</v>
+        <v>1.921184182167053</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -768,157 +753,148 @@
         <v>10</v>
       </c>
       <c r="I5">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L5">
-        <v>0.9164179563522339</v>
+        <v>0.934999942779541</v>
       </c>
       <c r="M5">
-        <v>0.904477596282959</v>
+        <v>0.9240000247955322</v>
       </c>
       <c r="N5">
-        <v>0.896969735622406</v>
+        <v>0.9294999837875366</v>
       </c>
       <c r="O5">
-        <v>0.9059550960858663</v>
+        <v>0.005499958992004395</v>
       </c>
       <c r="P5">
-        <v>0.008008144880462644</v>
-      </c>
-      <c r="Q5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:16">
       <c r="A6" s="1">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>139.0637479623159</v>
+        <v>150.27778673172</v>
       </c>
       <c r="C6">
-        <v>11.84118828485273</v>
+        <v>15.14872765541077</v>
       </c>
       <c r="D6">
-        <v>4.541523615519206</v>
+        <v>12.48603558540344</v>
       </c>
       <c r="E6">
-        <v>0.5061824543846188</v>
+        <v>0.8550000190734863</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H6">
         <v>10</v>
       </c>
       <c r="I6">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L6">
-        <v>0.9164179563522339</v>
+        <v>0.9319999814033508</v>
       </c>
       <c r="M6">
-        <v>0.8985074162483215</v>
+        <v>0.9259999990463257</v>
       </c>
       <c r="N6">
-        <v>0.8969696760177612</v>
+        <v>0.9289999902248383</v>
       </c>
       <c r="O6">
-        <v>0.9039650162061056</v>
+        <v>0.002999991178512573</v>
       </c>
       <c r="P6">
-        <v>0.008827908395781417</v>
-      </c>
-      <c r="Q6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:16">
       <c r="A7" s="1">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B7">
-        <v>53.04193234443665</v>
+        <v>136.3590759038925</v>
       </c>
       <c r="C7">
-        <v>8.771477526258465</v>
+        <v>0.814616322517395</v>
       </c>
       <c r="D7">
-        <v>5.394241571426392</v>
+        <v>11.60637199878693</v>
       </c>
       <c r="E7">
-        <v>1.038732197673116</v>
+        <v>0.2590881586074829</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
       </c>
       <c r="G7">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I7">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L7">
-        <v>0.9134328365325928</v>
+        <v>0.9269999861717224</v>
       </c>
       <c r="M7">
-        <v>0.9074626564979553</v>
+        <v>0.9299999475479126</v>
       </c>
       <c r="N7">
-        <v>0.8878787755966187</v>
+        <v>0.9284999668598175</v>
       </c>
       <c r="O7">
-        <v>0.9029247562090555</v>
+        <v>0.001499980688095093</v>
       </c>
       <c r="P7">
-        <v>0.01091472741616778</v>
-      </c>
-      <c r="Q7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:16">
       <c r="A8" s="1">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>133.3880138397217</v>
+        <v>181.310514330864</v>
       </c>
       <c r="C8">
-        <v>2.622285475432505</v>
+        <v>26.73155772686005</v>
       </c>
       <c r="D8">
-        <v>5.162713925043742</v>
+        <v>12.75997710227966</v>
       </c>
       <c r="E8">
-        <v>0.2269020638316955</v>
+        <v>0.07788753509521484</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G8">
         <v>20</v>
@@ -930,51 +906,48 @@
         <v>128</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L8">
-        <v>0.9074625968933105</v>
+        <v>0.9270000457763672</v>
       </c>
       <c r="M8">
-        <v>0.8895522356033325</v>
+        <v>0.9290000200271606</v>
       </c>
       <c r="N8">
-        <v>0.9060605764389038</v>
+        <v>0.9280000329017639</v>
       </c>
       <c r="O8">
-        <v>0.901025136311849</v>
+        <v>0.0009999871253967285</v>
       </c>
       <c r="P8">
-        <v>0.008132732355088356</v>
-      </c>
-      <c r="Q8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:16">
       <c r="A9" s="1">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>140.4387857913971</v>
+        <v>187.2225534915924</v>
       </c>
       <c r="C9">
-        <v>2.884168499334205</v>
+        <v>16.45252442359924</v>
       </c>
       <c r="D9">
-        <v>5.040391445159912</v>
+        <v>18.85060787200928</v>
       </c>
       <c r="E9">
-        <v>0.4871967504003464</v>
+        <v>6.266724586486816</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H9">
         <v>10</v>
@@ -983,48 +956,45 @@
         <v>128</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L9">
-        <v>0.8955223560333252</v>
+        <v>0.9250000715255737</v>
       </c>
       <c r="M9">
-        <v>0.9074626564979553</v>
+        <v>0.9309999942779541</v>
       </c>
       <c r="N9">
-        <v>0.8939393758773804</v>
+        <v>0.9280000329017639</v>
       </c>
       <c r="O9">
-        <v>0.8989747961362203</v>
+        <v>0.002999961376190186</v>
       </c>
       <c r="P9">
-        <v>0.006036515920283998</v>
-      </c>
-      <c r="Q9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="1">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>146.0741839408875</v>
+        <v>139.623464345932</v>
       </c>
       <c r="C10">
-        <v>4.042508879079694</v>
+        <v>23.12367415428162</v>
       </c>
       <c r="D10">
-        <v>15.03789019584656</v>
+        <v>13.59703326225281</v>
       </c>
       <c r="E10">
-        <v>6.291689010555989</v>
+        <v>0.5321846008300781</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10">
         <v>20</v>
@@ -1033,101 +1003,95 @@
         <v>10</v>
       </c>
       <c r="I10">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L10">
-        <v>0.9134328365325928</v>
+        <v>0.925000011920929</v>
       </c>
       <c r="M10">
-        <v>0.89552241563797</v>
+        <v>0.9269999861717224</v>
       </c>
       <c r="N10">
-        <v>0.8878788352012634</v>
+        <v>0.9259999990463257</v>
       </c>
       <c r="O10">
-        <v>0.8989446957906088</v>
+        <v>0.0009999871253967285</v>
       </c>
       <c r="P10">
-        <v>0.01070936497005477</v>
-      </c>
-      <c r="Q10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:16">
       <c r="A11" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B11">
-        <v>733.694678068161</v>
+        <v>193.3307368755341</v>
       </c>
       <c r="C11">
-        <v>879.9061287312825</v>
+        <v>22.13834095001221</v>
       </c>
       <c r="D11">
-        <v>5.900887330373128</v>
+        <v>15.0815190076828</v>
       </c>
       <c r="E11">
-        <v>2.327244264434575</v>
+        <v>1.950249314308167</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H11">
         <v>10</v>
       </c>
       <c r="I11">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J11" t="s">
         <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L11">
-        <v>0.9253730773925781</v>
+        <v>0.9210000038146973</v>
       </c>
       <c r="M11">
-        <v>0.8985075354576111</v>
+        <v>0.9290000200271606</v>
       </c>
       <c r="N11">
-        <v>0.8696969747543335</v>
+        <v>0.925000011920929</v>
       </c>
       <c r="O11">
-        <v>0.8978591958681742</v>
+        <v>0.004000008106231689</v>
       </c>
       <c r="P11">
-        <v>0.02273429654968474</v>
-      </c>
-      <c r="Q11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:16">
       <c r="A12" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12">
-        <v>74.07484992345174</v>
+        <v>141.1637037992477</v>
       </c>
       <c r="C12">
-        <v>20.03521622423804</v>
+        <v>0.1129332780838013</v>
       </c>
       <c r="D12">
-        <v>5.643171469370524</v>
+        <v>14.4291797876358</v>
       </c>
       <c r="E12">
-        <v>1.091181337797907</v>
+        <v>1.322872281074524</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -1136,7 +1100,7 @@
         <v>20</v>
       </c>
       <c r="H12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I12">
         <v>256</v>
@@ -1145,48 +1109,45 @@
         <v>18</v>
       </c>
       <c r="K12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L12">
-        <v>0.8955223560333252</v>
+        <v>0.9249998331069946</v>
       </c>
       <c r="M12">
-        <v>0.9134328365325928</v>
+        <v>0.921999990940094</v>
       </c>
       <c r="N12">
-        <v>0.8696969151496887</v>
+        <v>0.9234999120235443</v>
       </c>
       <c r="O12">
-        <v>0.8928840359052023</v>
+        <v>0.001499921083450317</v>
       </c>
       <c r="P12">
-        <v>0.01795231191475042</v>
-      </c>
-      <c r="Q12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:16">
       <c r="A13" s="1">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>125.287312189738</v>
+        <v>111.5190763473511</v>
       </c>
       <c r="C13">
-        <v>2.848083827545802</v>
+        <v>1.212055206298828</v>
       </c>
       <c r="D13">
-        <v>5.21040137608846</v>
+        <v>11.61174273490906</v>
       </c>
       <c r="E13">
-        <v>0.3132591712494442</v>
+        <v>0.08298683166503906</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G13">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H13">
         <v>10</v>
@@ -1198,45 +1159,42 @@
         <v>18</v>
       </c>
       <c r="K13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L13">
-        <v>0.9194030165672302</v>
+        <v>0.9319999814033508</v>
       </c>
       <c r="M13">
-        <v>0.9014924764633179</v>
+        <v>0.9140000343322754</v>
       </c>
       <c r="N13">
-        <v>0.8515151143074036</v>
+        <v>0.9230000078678131</v>
       </c>
       <c r="O13">
-        <v>0.8908035357793173</v>
+        <v>0.00899997353553772</v>
       </c>
       <c r="P13">
-        <v>0.02872724500098014</v>
-      </c>
-      <c r="Q13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:16">
       <c r="A14" s="1">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>130.9250098864237</v>
+        <v>115.1637585163116</v>
       </c>
       <c r="C14">
-        <v>2.928556346320716</v>
+        <v>3.874695301055908</v>
       </c>
       <c r="D14">
-        <v>4.804123481114705</v>
+        <v>10.71052861213684</v>
       </c>
       <c r="E14">
-        <v>0.216546873076932</v>
+        <v>0.4466373920440674</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <v>25</v>
@@ -1248,51 +1206,48 @@
         <v>128</v>
       </c>
       <c r="J14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L14">
-        <v>0.8895522952079773</v>
+        <v>0.9230000376701355</v>
       </c>
       <c r="M14">
-        <v>0.8746268153190613</v>
+        <v>0.9209998846054077</v>
       </c>
       <c r="N14">
-        <v>0.9060606360435486</v>
+        <v>0.9219999611377716</v>
       </c>
       <c r="O14">
-        <v>0.8900799155235291</v>
+        <v>0.001000076532363892</v>
       </c>
       <c r="P14">
-        <v>0.01283822570121066</v>
-      </c>
-      <c r="Q14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:16">
       <c r="A15" s="1">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B15">
-        <v>66.49570528666179</v>
+        <v>68.54301083087921</v>
       </c>
       <c r="C15">
-        <v>12.04353351159397</v>
+        <v>8.528471350669861</v>
       </c>
       <c r="D15">
-        <v>8.22185722986857</v>
+        <v>11.91691446304321</v>
       </c>
       <c r="E15">
-        <v>4.701438716648958</v>
+        <v>0.7704586982727051</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
       </c>
       <c r="G15">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H15">
         <v>5</v>
@@ -1304,42 +1259,39 @@
         <v>18</v>
       </c>
       <c r="K15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L15">
-        <v>0.8985074758529663</v>
+        <v>0.9240000247955322</v>
       </c>
       <c r="M15">
-        <v>0.8865671753883362</v>
+        <v>0.9189999103546143</v>
       </c>
       <c r="N15">
-        <v>0.8787878751754761</v>
+        <v>0.9214999675750732</v>
       </c>
       <c r="O15">
-        <v>0.8879541754722595</v>
+        <v>0.002500057220458984</v>
       </c>
       <c r="P15">
-        <v>0.008110013959894309</v>
-      </c>
-      <c r="Q15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:16">
       <c r="A16" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B16">
-        <v>74.36285765965779</v>
+        <v>142.9282509088516</v>
       </c>
       <c r="C16">
-        <v>14.00122835394506</v>
+        <v>0.9941028356552124</v>
       </c>
       <c r="D16">
-        <v>11.3113473256429</v>
+        <v>15.41558229923248</v>
       </c>
       <c r="E16">
-        <v>6.680864780809817</v>
+        <v>2.586351752281189</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
@@ -1348,51 +1300,48 @@
         <v>20</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L16">
-        <v>0.9074625968933105</v>
+        <v>0.906999945640564</v>
       </c>
       <c r="M16">
-        <v>0.8716417551040649</v>
+        <v>0.9330000281333923</v>
       </c>
       <c r="N16">
-        <v>0.8787878751754761</v>
+        <v>0.9199999868869781</v>
       </c>
       <c r="O16">
-        <v>0.8859640757242838</v>
+        <v>0.01300004124641418</v>
       </c>
       <c r="P16">
-        <v>0.01547915948105867</v>
-      </c>
-      <c r="Q16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:16">
       <c r="A17" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B17">
-        <v>74.33030064900716</v>
+        <v>70.08843576908112</v>
       </c>
       <c r="C17">
-        <v>17.05531198814253</v>
+        <v>3.660466074943542</v>
       </c>
       <c r="D17">
-        <v>5.555164575576782</v>
+        <v>14.51486754417419</v>
       </c>
       <c r="E17">
-        <v>1.672171763965501</v>
+        <v>2.431852102279663</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -1404,48 +1353,45 @@
         <v>5</v>
       </c>
       <c r="I17">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L17">
-        <v>0.886567234992981</v>
+        <v>0.9169999957084656</v>
       </c>
       <c r="M17">
-        <v>0.8776119947433472</v>
+        <v>0.9150000214576721</v>
       </c>
       <c r="N17">
-        <v>0.8757575154304504</v>
+        <v>0.9160000085830688</v>
       </c>
       <c r="O17">
-        <v>0.8799789150555929</v>
+        <v>0.0009999871253967285</v>
       </c>
       <c r="P17">
-        <v>0.004719762923320736</v>
-      </c>
-      <c r="Q17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:16">
       <c r="A18" s="1">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18">
-        <v>66.62978466351827</v>
+        <v>85.05287992954254</v>
       </c>
       <c r="C18">
-        <v>17.38780785568654</v>
+        <v>8.842670083045959</v>
       </c>
       <c r="D18">
-        <v>8.318903843561808</v>
+        <v>17.13321840763092</v>
       </c>
       <c r="E18">
-        <v>4.423451633198773</v>
+        <v>2.617046713829041</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -1457,101 +1403,95 @@
         <v>5</v>
       </c>
       <c r="I18">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J18" t="s">
         <v>18</v>
       </c>
       <c r="K18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L18">
-        <v>0.8686566948890686</v>
+        <v>0.9319999814033508</v>
       </c>
       <c r="M18">
-        <v>0.8746268749237061</v>
+        <v>0.8989999890327454</v>
       </c>
       <c r="N18">
-        <v>0.8939393162727356</v>
+        <v>0.9154999852180481</v>
       </c>
       <c r="O18">
-        <v>0.8790742953618368</v>
+        <v>0.01649999618530273</v>
       </c>
       <c r="P18">
-        <v>0.01079003853631027</v>
-      </c>
-      <c r="Q18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:16">
       <c r="A19" s="1">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>86.62878847122192</v>
+      </c>
+      <c r="C19">
+        <v>13.71841716766357</v>
+      </c>
+      <c r="D19">
+        <v>14.19310760498047</v>
+      </c>
+      <c r="E19">
+        <v>2.428851366043091</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19">
+        <v>20</v>
+      </c>
+      <c r="H19">
         <v>5</v>
-      </c>
-      <c r="B19">
-        <v>115.3827340602875</v>
-      </c>
-      <c r="C19">
-        <v>2.938009680901168</v>
-      </c>
-      <c r="D19">
-        <v>10.52469603220622</v>
-      </c>
-      <c r="E19">
-        <v>3.925206061234818</v>
-      </c>
-      <c r="F19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19">
-        <v>25</v>
-      </c>
-      <c r="H19">
-        <v>10</v>
       </c>
       <c r="I19">
         <v>256</v>
       </c>
       <c r="J19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L19">
+        <v>0.9160000085830688</v>
+      </c>
+      <c r="M19">
+        <v>0.9110000729560852</v>
+      </c>
+      <c r="N19">
+        <v>0.913500040769577</v>
+      </c>
+      <c r="O19">
+        <v>0.002499967813491821</v>
+      </c>
+      <c r="P19">
         <v>18</v>
       </c>
-      <c r="K19" t="s">
-        <v>37</v>
-      </c>
-      <c r="L19">
-        <v>0.8029851317405701</v>
-      </c>
-      <c r="M19">
-        <v>0.904477596282959</v>
-      </c>
-      <c r="N19">
-        <v>0.9060606360435486</v>
-      </c>
-      <c r="O19">
-        <v>0.8711744546890259</v>
-      </c>
-      <c r="P19">
-        <v>0.04822146359487307</v>
-      </c>
-      <c r="Q19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="1">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>131.4374632835388</v>
+        <v>103.2003771066666</v>
       </c>
       <c r="C20">
-        <v>3.014324335015929</v>
+        <v>3.280528664588928</v>
       </c>
       <c r="D20">
-        <v>9.672802925109863</v>
+        <v>12.4791522026062</v>
       </c>
       <c r="E20">
-        <v>6.497336663406538</v>
+        <v>0.8874263763427734</v>
       </c>
       <c r="F20" t="s">
         <v>16</v>
@@ -1560,157 +1500,148 @@
         <v>25</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I20">
         <v>256</v>
       </c>
       <c r="J20" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" t="s">
+        <v>37</v>
+      </c>
+      <c r="L20">
+        <v>0.9210000038146973</v>
+      </c>
+      <c r="M20">
+        <v>0.9049999713897705</v>
+      </c>
+      <c r="N20">
+        <v>0.9129999876022339</v>
+      </c>
+      <c r="O20">
+        <v>0.008000016212463379</v>
+      </c>
+      <c r="P20">
         <v>19</v>
       </c>
-      <c r="K20" t="s">
-        <v>38</v>
-      </c>
-      <c r="L20">
-        <v>0.8686566948890686</v>
-      </c>
-      <c r="M20">
-        <v>0.8507463335990906</v>
-      </c>
-      <c r="N20">
-        <v>0.8939393758773804</v>
-      </c>
-      <c r="O20">
-        <v>0.8711141347885132</v>
-      </c>
-      <c r="P20">
-        <v>0.01771889732193794</v>
-      </c>
-      <c r="Q20">
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="1">
-        <v>6</v>
-      </c>
       <c r="B21">
-        <v>112.6923964818319</v>
+        <v>112.3674980401993</v>
       </c>
       <c r="C21">
-        <v>4.399059745862806</v>
+        <v>1.912895798683167</v>
       </c>
       <c r="D21">
-        <v>4.189464012781779</v>
+        <v>13.88630616664886</v>
       </c>
       <c r="E21">
-        <v>0.3503958701721298</v>
+        <v>0.4235292673110962</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21">
         <v>25</v>
       </c>
       <c r="H21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I21">
         <v>128</v>
       </c>
       <c r="J21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L21">
-        <v>0.8656716346740723</v>
+        <v>0.9079999327659607</v>
       </c>
       <c r="M21">
-        <v>0.8716418147087097</v>
+        <v>0.9169999957084656</v>
       </c>
       <c r="N21">
-        <v>0.8696969747543335</v>
+        <v>0.9124999642372131</v>
       </c>
       <c r="O21">
-        <v>0.8690034747123718</v>
+        <v>0.004500031471252441</v>
       </c>
       <c r="P21">
-        <v>0.002486157563074196</v>
-      </c>
-      <c r="Q21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:16">
       <c r="A22" s="1">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>64.02316840489705</v>
+        <v>110.3258522748947</v>
       </c>
       <c r="C22">
-        <v>15.66647370593406</v>
+        <v>0.8902684450149536</v>
       </c>
       <c r="D22">
-        <v>9.666007916132608</v>
+        <v>11.02676975727081</v>
       </c>
       <c r="E22">
-        <v>6.74894285778613</v>
+        <v>0.1997205018997192</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22">
         <v>25</v>
       </c>
       <c r="H22">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I22">
         <v>128</v>
       </c>
       <c r="J22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L22">
-        <v>0.8417910933494568</v>
+        <v>0.906999945640564</v>
       </c>
       <c r="M22">
-        <v>0.8805969953536987</v>
+        <v>0.9139999151229858</v>
       </c>
       <c r="N22">
-        <v>0.8818181753158569</v>
+        <v>0.9104999303817749</v>
       </c>
       <c r="O22">
-        <v>0.8680687546730042</v>
+        <v>0.003499984741210938</v>
       </c>
       <c r="P22">
-        <v>0.01858779946813298</v>
-      </c>
-      <c r="Q22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:16">
       <c r="A23" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23">
-        <v>65.43442940711975</v>
+        <v>81.08935630321503</v>
       </c>
       <c r="C23">
-        <v>15.62040132981878</v>
+        <v>18.50767362117767</v>
       </c>
       <c r="D23">
-        <v>5.197110017140706</v>
+        <v>19.50814354419708</v>
       </c>
       <c r="E23">
-        <v>1.205024106710354</v>
+        <v>5.129084944725037</v>
       </c>
       <c r="F23" t="s">
         <v>16</v>
@@ -1722,157 +1653,148 @@
         <v>5</v>
       </c>
       <c r="I23">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J23" t="s">
         <v>18</v>
       </c>
       <c r="K23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L23">
-        <v>0.8298507332801819</v>
+        <v>0.9049999117851257</v>
       </c>
       <c r="M23">
-        <v>0.880596935749054</v>
+        <v>0.8939999341964722</v>
       </c>
       <c r="N23">
-        <v>0.8818182349205017</v>
+        <v>0.899499922990799</v>
       </c>
       <c r="O23">
-        <v>0.8640886346499125</v>
+        <v>0.005499988794326782</v>
       </c>
       <c r="P23">
-        <v>0.02421498586370427</v>
-      </c>
-      <c r="Q23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:16">
       <c r="A24" s="1">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B24">
-        <v>992.8292651176453</v>
+        <v>98.84335350990295</v>
       </c>
       <c r="C24">
-        <v>1245.974226839766</v>
+        <v>6.773154020309448</v>
       </c>
       <c r="D24">
-        <v>4.191378911336263</v>
+        <v>22.12243497371674</v>
       </c>
       <c r="E24">
-        <v>0.1403756232513582</v>
+        <v>7.694762587547302</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24">
         <v>25</v>
       </c>
       <c r="H24">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I24">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J24" t="s">
         <v>18</v>
       </c>
       <c r="K24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L24">
-        <v>0.8716418147087097</v>
+        <v>0.9129999279975891</v>
       </c>
       <c r="M24">
-        <v>0.89552241563797</v>
+        <v>0.8819999098777771</v>
       </c>
       <c r="N24">
-        <v>0.8242424726486206</v>
+        <v>0.8974999189376831</v>
       </c>
       <c r="O24">
-        <v>0.8638022343317667</v>
+        <v>0.01550000905990601</v>
       </c>
       <c r="P24">
-        <v>0.02962320974625736</v>
-      </c>
-      <c r="Q24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:16">
       <c r="A25" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B25">
-        <v>60.55417084693909</v>
+        <v>112.8342931270599</v>
       </c>
       <c r="C25">
-        <v>12.28426764377543</v>
+        <v>6.430818557739258</v>
       </c>
       <c r="D25">
-        <v>5.947096586227417</v>
+        <v>771.8749134540558</v>
       </c>
       <c r="E25">
-        <v>1.567065480771697</v>
+        <v>761.3899502754211</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G25">
         <v>20</v>
       </c>
       <c r="H25">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I25">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L25">
-        <v>0.8776119351387024</v>
+        <v>0.8490000367164612</v>
       </c>
       <c r="M25">
-        <v>0.8238806128501892</v>
+        <v>0.937000036239624</v>
       </c>
       <c r="N25">
-        <v>0.8878788352012634</v>
+        <v>0.8930000364780426</v>
       </c>
       <c r="O25">
-        <v>0.8631237943967184</v>
+        <v>0.04399999976158142</v>
       </c>
       <c r="P25">
-        <v>0.02806388880921575</v>
-      </c>
-      <c r="Q25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:16">
       <c r="A26" s="1">
         <v>1</v>
       </c>
       <c r="B26">
-        <v>56.7287171681722</v>
+        <v>56.08218157291412</v>
       </c>
       <c r="C26">
-        <v>9.540145426381693</v>
+        <v>2.893380761146545</v>
       </c>
       <c r="D26">
-        <v>6.073423385620117</v>
+        <v>11.26058793067932</v>
       </c>
       <c r="E26">
-        <v>3.233729008795648</v>
+        <v>0.9836664199829102</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G26">
         <v>25</v>
@@ -1884,48 +1806,45 @@
         <v>256</v>
       </c>
       <c r="J26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L26">
-        <v>0.8985074162483215</v>
+        <v>0.8859999775886536</v>
       </c>
       <c r="M26">
-        <v>0.8059701323509216</v>
+        <v>0.8819999694824219</v>
       </c>
       <c r="N26">
-        <v>0.8787878751754761</v>
+        <v>0.8839999735355377</v>
       </c>
       <c r="O26">
-        <v>0.8610884745915731</v>
+        <v>0.002000004053115845</v>
       </c>
       <c r="P26">
-        <v>0.03979730990531141</v>
-      </c>
-      <c r="Q26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:16">
       <c r="A27" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27">
-        <v>46.43642870585123</v>
+        <v>58.81357645988464</v>
       </c>
       <c r="C27">
-        <v>7.561643605093507</v>
+        <v>3.650204420089722</v>
       </c>
       <c r="D27">
-        <v>5.112329403559367</v>
+        <v>11.54615926742554</v>
       </c>
       <c r="E27">
-        <v>1.254999875879873</v>
+        <v>0.1006989479064941</v>
       </c>
       <c r="F27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G27">
         <v>20</v>
@@ -1940,45 +1859,42 @@
         <v>18</v>
       </c>
       <c r="K27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L27">
-        <v>0.8537313342094421</v>
+        <v>0.8709999918937683</v>
       </c>
       <c r="M27">
-        <v>0.8776119351387024</v>
+        <v>0.8939999938011169</v>
       </c>
       <c r="N27">
-        <v>0.8484849333763123</v>
+        <v>0.8824999928474426</v>
       </c>
       <c r="O27">
-        <v>0.8599427342414856</v>
+        <v>0.01150000095367432</v>
       </c>
       <c r="P27">
-        <v>0.01267626852784687</v>
-      </c>
-      <c r="Q27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:16">
       <c r="A28" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B28">
-        <v>68.62597346305847</v>
+        <v>59.57585680484772</v>
       </c>
       <c r="C28">
-        <v>13.95137037377635</v>
+        <v>0.6418379545211792</v>
       </c>
       <c r="D28">
-        <v>7.028938372929891</v>
+        <v>11.83613276481628</v>
       </c>
       <c r="E28">
-        <v>3.453449339573602</v>
+        <v>1.074345111846924</v>
       </c>
       <c r="F28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G28">
         <v>20</v>
@@ -1987,51 +1903,48 @@
         <v>5</v>
       </c>
       <c r="I28">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L28">
-        <v>0.8298507928848267</v>
+        <v>0.8960000872612</v>
       </c>
       <c r="M28">
-        <v>0.8626866340637207</v>
+        <v>0.8540000319480896</v>
       </c>
       <c r="N28">
-        <v>0.8818181753158569</v>
+        <v>0.8750000596046448</v>
       </c>
       <c r="O28">
-        <v>0.8581185340881348</v>
+        <v>0.02100002765655518</v>
       </c>
       <c r="P28">
-        <v>0.02146008484331551</v>
-      </c>
-      <c r="Q28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:16">
       <c r="A29" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B29">
-        <v>49.26799861590067</v>
+        <v>55.76097989082336</v>
       </c>
       <c r="C29">
-        <v>12.35363734708296</v>
+        <v>2.686948776245117</v>
       </c>
       <c r="D29">
-        <v>5.058491468429565</v>
+        <v>10.45479798316956</v>
       </c>
       <c r="E29">
-        <v>1.325063356764046</v>
+        <v>0.2495784759521484</v>
       </c>
       <c r="F29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G29">
         <v>25</v>
@@ -2040,104 +1953,98 @@
         <v>5</v>
       </c>
       <c r="I29">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L29">
-        <v>0.9164179563522339</v>
+        <v>0.8919999599456787</v>
       </c>
       <c r="M29">
-        <v>0.8029851317405701</v>
+        <v>0.8510000705718994</v>
       </c>
       <c r="N29">
-        <v>0.8030303120613098</v>
+        <v>0.8715000152587891</v>
       </c>
       <c r="O29">
-        <v>0.8408111333847046</v>
+        <v>0.02049994468688965</v>
       </c>
       <c r="P29">
-        <v>0.05346210040609972</v>
-      </c>
-      <c r="Q29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:16">
       <c r="A30" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B30">
-        <v>113.65762702624</v>
+        <v>52.34040093421936</v>
       </c>
       <c r="C30">
-        <v>0.8220505812669434</v>
+        <v>1.535679340362549</v>
       </c>
       <c r="D30">
-        <v>3.905224720637003</v>
+        <v>10.10178458690643</v>
       </c>
       <c r="E30">
-        <v>0.01385025860172755</v>
+        <v>0.07559406757354736</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G30">
         <v>25</v>
       </c>
       <c r="H30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I30">
         <v>256</v>
       </c>
       <c r="J30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L30">
-        <v>0.9074627161026001</v>
+        <v>0.8380000591278076</v>
       </c>
       <c r="M30">
-        <v>0.6955223679542542</v>
+        <v>0.8940001130104065</v>
       </c>
       <c r="N30">
-        <v>0.8393939733505249</v>
+        <v>0.8660000860691071</v>
       </c>
       <c r="O30">
-        <v>0.8141263524691263</v>
+        <v>0.02800002694129944</v>
       </c>
       <c r="P30">
-        <v>0.08834974926229308</v>
-      </c>
-      <c r="Q30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:16">
       <c r="A31" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B31">
-        <v>39.81176551183065</v>
+        <v>59.78808236122131</v>
       </c>
       <c r="C31">
-        <v>0.4984907894750415</v>
+        <v>2.484103918075562</v>
       </c>
       <c r="D31">
-        <v>4.125336011250814</v>
+        <v>12.01153135299683</v>
       </c>
       <c r="E31">
-        <v>0.1356334921386906</v>
+        <v>1.047560214996338</v>
       </c>
       <c r="F31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G31">
         <v>20</v>
@@ -2146,54 +2053,51 @@
         <v>5</v>
       </c>
       <c r="I31">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L31">
-        <v>0.832835853099823</v>
+        <v>0.8409999012947083</v>
       </c>
       <c r="M31">
-        <v>0.8208954930305481</v>
+        <v>0.887999951839447</v>
       </c>
       <c r="N31">
-        <v>0.7666667103767395</v>
+        <v>0.8644999265670776</v>
       </c>
       <c r="O31">
-        <v>0.8067993521690369</v>
+        <v>0.02350002527236938</v>
       </c>
       <c r="P31">
-        <v>0.02879368857426483</v>
-      </c>
-      <c r="Q31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:16">
       <c r="A32" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B32">
-        <v>61.74911745389303</v>
+        <v>56.04004621505737</v>
       </c>
       <c r="C32">
-        <v>15.04025513510453</v>
+        <v>0.2442131042480469</v>
       </c>
       <c r="D32">
-        <v>5.119652668635051</v>
+        <v>12.55375599861145</v>
       </c>
       <c r="E32">
-        <v>1.152323703920358</v>
+        <v>0.0222628116607666</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G32">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H32">
         <v>5</v>
@@ -2202,48 +2106,45 @@
         <v>128</v>
       </c>
       <c r="J32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L32">
-        <v>0.8298507332801819</v>
+        <v>0.8349999189376831</v>
       </c>
       <c r="M32">
-        <v>0.7970149517059326</v>
+        <v>0.8680000305175781</v>
       </c>
       <c r="N32">
-        <v>0.7848484516143799</v>
+        <v>0.8514999747276306</v>
       </c>
       <c r="O32">
-        <v>0.8039047122001648</v>
+        <v>0.01650005578994751</v>
       </c>
       <c r="P32">
-        <v>0.01900706778250232</v>
-      </c>
-      <c r="Q32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:16">
       <c r="A33" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B33">
-        <v>57.46216837565104</v>
+        <v>55.50199258327484</v>
       </c>
       <c r="C33">
-        <v>11.97215545140205</v>
+        <v>2.926184773445129</v>
       </c>
       <c r="D33">
-        <v>9.077148278554281</v>
+        <v>10.69364142417908</v>
       </c>
       <c r="E33">
-        <v>6.496483655854372</v>
+        <v>0.212160587310791</v>
       </c>
       <c r="F33" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G33">
         <v>25</v>
@@ -2258,24 +2159,21 @@
         <v>18</v>
       </c>
       <c r="K33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L33">
-        <v>0.8059701323509216</v>
+        <v>0.8259999752044678</v>
       </c>
       <c r="M33">
-        <v>0.8059701323509216</v>
+        <v>0.8690000176429749</v>
       </c>
       <c r="N33">
-        <v>0.7878788113594055</v>
+        <v>0.8474999964237213</v>
       </c>
       <c r="O33">
-        <v>0.7999396920204163</v>
+        <v>0.02150002121925354</v>
       </c>
       <c r="P33">
-        <v>0.008528330502482386</v>
-      </c>
-      <c r="Q33">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update notebook for q2 and q1
</commit_message>
<xml_diff>
--- a/output_Q2/DF_Full_Result.xlsx
+++ b/output_Q2/DF_Full_Result.xlsx
@@ -61,88 +61,100 @@
     <t>rank_test_score</t>
   </si>
   <si>
+    <t>adam</t>
+  </si>
+  <si>
     <t>rmsprop</t>
   </si>
   <si>
-    <t>adam</t>
-  </si>
-  <si>
     <t>sigmoid</t>
   </si>
   <si>
     <t>softmax</t>
   </si>
   <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
   </si>
   <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
   </si>
   <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
   </si>
   <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 10, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
   </si>
   <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
@@ -154,19 +166,7 @@
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
   </si>
   <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 25, 'epochs': 5, 'hidUnit': 128, 'outActivation': 'softmax'}</t>
   </si>
 </sst>
 </file>
@@ -579,25 +579,25 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B2">
-        <v>112.3461164236069</v>
+        <v>135.647961139679</v>
       </c>
       <c r="C2">
-        <v>1.52138888835907</v>
+        <v>0.451862096786499</v>
       </c>
       <c r="D2">
-        <v>10.59885251522064</v>
+        <v>11.1400398015976</v>
       </c>
       <c r="E2">
-        <v>0.3773878812789917</v>
+        <v>0.08981120586395264</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -612,16 +612,16 @@
         <v>19</v>
       </c>
       <c r="L2">
-        <v>0.9359999895095825</v>
+        <v>0.9350000023841858</v>
       </c>
       <c r="M2">
-        <v>0.9320000410079956</v>
+        <v>0.9330000281333923</v>
       </c>
       <c r="N2">
         <v>0.9340000152587891</v>
       </c>
       <c r="O2">
-        <v>0.001999974250793457</v>
+        <v>0.0009999871253967285</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -629,22 +629,22 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>138.8890740871429</v>
+        <v>128.6528992652893</v>
       </c>
       <c r="C3">
-        <v>6.420517921447754</v>
+        <v>1.186521768569946</v>
       </c>
       <c r="D3">
-        <v>14.20784938335419</v>
+        <v>15.51725471019745</v>
       </c>
       <c r="E3">
-        <v>1.375924229621887</v>
+        <v>0.3828204870223999</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>25</v>
@@ -653,7 +653,7 @@
         <v>10</v>
       </c>
       <c r="I3">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -662,16 +662,16 @@
         <v>20</v>
       </c>
       <c r="L3">
-        <v>0.9309999942779541</v>
+        <v>0.9339999556541443</v>
       </c>
       <c r="M3">
-        <v>0.9300000071525574</v>
+        <v>0.9319999814033508</v>
       </c>
       <c r="N3">
-        <v>0.9305000007152557</v>
+        <v>0.9329999685287476</v>
       </c>
       <c r="O3">
-        <v>0.0004999935626983643</v>
+        <v>0.0009999871253967285</v>
       </c>
       <c r="P3">
         <v>2</v>
@@ -679,31 +679,31 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B4">
-        <v>165.5413037538528</v>
+        <v>142.6886615753174</v>
       </c>
       <c r="C4">
-        <v>19.59417903423309</v>
+        <v>2.287525177001953</v>
       </c>
       <c r="D4">
-        <v>30.81350088119507</v>
+        <v>12.21938562393188</v>
       </c>
       <c r="E4">
-        <v>16.31952834129333</v>
+        <v>0.1852486133575439</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>10</v>
       </c>
       <c r="I4">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
@@ -712,66 +712,66 @@
         <v>21</v>
       </c>
       <c r="L4">
-        <v>0.9300000071525574</v>
+        <v>0.9360001087188721</v>
       </c>
       <c r="M4">
-        <v>0.9309999942779541</v>
+        <v>0.9239999651908875</v>
       </c>
       <c r="N4">
-        <v>0.9305000007152557</v>
+        <v>0.9300000369548798</v>
       </c>
       <c r="O4">
-        <v>0.0004999935626983643</v>
+        <v>0.00600007176399231</v>
       </c>
       <c r="P4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>147.7576627731323</v>
+        <v>67.48369705677032</v>
       </c>
       <c r="C5">
-        <v>0.3653357028961182</v>
+        <v>10.3750923871994</v>
       </c>
       <c r="D5">
-        <v>16.03926026821136</v>
+        <v>12.40147221088409</v>
       </c>
       <c r="E5">
-        <v>1.921184182167053</v>
+        <v>1.820365071296692</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I5">
         <v>128</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K5" t="s">
         <v>22</v>
       </c>
       <c r="L5">
-        <v>0.934999942779541</v>
+        <v>0.9299999475479126</v>
       </c>
       <c r="M5">
-        <v>0.9240000247955322</v>
+        <v>0.9290000200271606</v>
       </c>
       <c r="N5">
         <v>0.9294999837875366</v>
       </c>
       <c r="O5">
-        <v>0.005499958992004395</v>
+        <v>0.0004999637603759766</v>
       </c>
       <c r="P5">
         <v>4</v>
@@ -779,22 +779,22 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>150.27778673172</v>
+        <v>126.6618014574051</v>
       </c>
       <c r="C6">
-        <v>15.14872765541077</v>
+        <v>0.7417563199996948</v>
       </c>
       <c r="D6">
-        <v>12.48603558540344</v>
+        <v>15.48221921920776</v>
       </c>
       <c r="E6">
-        <v>0.8550000190734863</v>
+        <v>0.5201008319854736</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>25</v>
@@ -806,7 +806,7 @@
         <v>128</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" t="s">
         <v>23</v>
@@ -815,13 +815,13 @@
         <v>0.9319999814033508</v>
       </c>
       <c r="M6">
-        <v>0.9259999990463257</v>
+        <v>0.925000011920929</v>
       </c>
       <c r="N6">
-        <v>0.9289999902248383</v>
+        <v>0.9284999966621399</v>
       </c>
       <c r="O6">
-        <v>0.002999991178512573</v>
+        <v>0.003499984741210938</v>
       </c>
       <c r="P6">
         <v>5</v>
@@ -829,25 +829,25 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="1">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B7">
-        <v>136.3590759038925</v>
+        <v>126.0431751012802</v>
       </c>
       <c r="C7">
-        <v>0.814616322517395</v>
+        <v>2.35762083530426</v>
       </c>
       <c r="D7">
-        <v>11.60637199878693</v>
+        <v>17.29030156135559</v>
       </c>
       <c r="E7">
-        <v>0.2590881586074829</v>
+        <v>0.8555421829223633</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H7">
         <v>10</v>
@@ -862,16 +862,16 @@
         <v>24</v>
       </c>
       <c r="L7">
-        <v>0.9269999861717224</v>
+        <v>0.9290000796318054</v>
       </c>
       <c r="M7">
-        <v>0.9299999475479126</v>
+        <v>0.9270000457763672</v>
       </c>
       <c r="N7">
-        <v>0.9284999668598175</v>
+        <v>0.9280000627040863</v>
       </c>
       <c r="O7">
-        <v>0.001499980688095093</v>
+        <v>0.001000016927719116</v>
       </c>
       <c r="P7">
         <v>6</v>
@@ -882,19 +882,19 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>181.310514330864</v>
+        <v>130.290415763855</v>
       </c>
       <c r="C8">
-        <v>26.73155772686005</v>
+        <v>0.2203841209411621</v>
       </c>
       <c r="D8">
-        <v>12.75997710227966</v>
+        <v>12.67466580867767</v>
       </c>
       <c r="E8">
-        <v>0.07788753509521484</v>
+        <v>0.3614319562911987</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8">
         <v>20</v>
@@ -912,16 +912,16 @@
         <v>25</v>
       </c>
       <c r="L8">
-        <v>0.9270000457763672</v>
+        <v>0.9220001101493835</v>
       </c>
       <c r="M8">
-        <v>0.9290000200271606</v>
+        <v>0.9329999685287476</v>
       </c>
       <c r="N8">
-        <v>0.9280000329017639</v>
+        <v>0.9275000393390656</v>
       </c>
       <c r="O8">
-        <v>0.0009999871253967285</v>
+        <v>0.005499929189682007</v>
       </c>
       <c r="P8">
         <v>7</v>
@@ -929,75 +929,75 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>187.2225534915924</v>
+        <v>66.94822025299072</v>
       </c>
       <c r="C9">
-        <v>16.45252442359924</v>
+        <v>10.46286654472351</v>
       </c>
       <c r="D9">
-        <v>18.85060787200928</v>
+        <v>12.28138518333435</v>
       </c>
       <c r="E9">
-        <v>6.266724586486816</v>
+        <v>0.6114089488983154</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I9">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K9" t="s">
         <v>26</v>
       </c>
       <c r="L9">
-        <v>0.9250000715255737</v>
+        <v>0.9169999957084656</v>
       </c>
       <c r="M9">
-        <v>0.9309999942779541</v>
+        <v>0.9340000152587891</v>
       </c>
       <c r="N9">
-        <v>0.9280000329017639</v>
+        <v>0.9255000054836273</v>
       </c>
       <c r="O9">
-        <v>0.002999961376190186</v>
+        <v>0.008500009775161743</v>
       </c>
       <c r="P9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="1">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>139.623464345932</v>
+        <v>123.1933196783066</v>
       </c>
       <c r="C10">
-        <v>23.12367415428162</v>
+        <v>0.3570035696029663</v>
       </c>
       <c r="D10">
-        <v>13.59703326225281</v>
+        <v>10.19103515148163</v>
       </c>
       <c r="E10">
-        <v>0.5321846008300781</v>
+        <v>0.07597649097442627</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G10">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H10">
         <v>10</v>
@@ -1006,22 +1006,22 @@
         <v>256</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K10" t="s">
         <v>27</v>
       </c>
       <c r="L10">
-        <v>0.925000011920929</v>
+        <v>0.9299999475479126</v>
       </c>
       <c r="M10">
-        <v>0.9269999861717224</v>
+        <v>0.9210000038146973</v>
       </c>
       <c r="N10">
-        <v>0.9259999990463257</v>
+        <v>0.9254999756813049</v>
       </c>
       <c r="O10">
-        <v>0.0009999871253967285</v>
+        <v>0.004499971866607666</v>
       </c>
       <c r="P10">
         <v>9</v>
@@ -1029,25 +1029,25 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="1">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>137.9967179298401</v>
+      </c>
+      <c r="C11">
+        <v>0.942446231842041</v>
+      </c>
+      <c r="D11">
+        <v>11.34811043739319</v>
+      </c>
+      <c r="E11">
+        <v>0.1016659736633301</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
         <v>20</v>
-      </c>
-      <c r="B11">
-        <v>193.3307368755341</v>
-      </c>
-      <c r="C11">
-        <v>22.13834095001221</v>
-      </c>
-      <c r="D11">
-        <v>15.0815190076828</v>
-      </c>
-      <c r="E11">
-        <v>1.950249314308167</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11">
-        <v>25</v>
       </c>
       <c r="H11">
         <v>10</v>
@@ -1062,16 +1062,16 @@
         <v>28</v>
       </c>
       <c r="L11">
+        <v>0.9280000329017639</v>
+      </c>
+      <c r="M11">
         <v>0.9210000038146973</v>
       </c>
-      <c r="M11">
-        <v>0.9290000200271606</v>
-      </c>
       <c r="N11">
-        <v>0.925000011920929</v>
+        <v>0.9245000183582306</v>
       </c>
       <c r="O11">
-        <v>0.004000008106231689</v>
+        <v>0.003500014543533325</v>
       </c>
       <c r="P11">
         <v>10</v>
@@ -1079,22 +1079,22 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12">
-        <v>141.1637037992477</v>
+        <v>133.3673646450043</v>
       </c>
       <c r="C12">
-        <v>0.1129332780838013</v>
+        <v>0.3674001693725586</v>
       </c>
       <c r="D12">
-        <v>14.4291797876358</v>
+        <v>11.22293758392334</v>
       </c>
       <c r="E12">
-        <v>1.322872281074524</v>
+        <v>0.06707763671875</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12">
         <v>20</v>
@@ -1103,7 +1103,7 @@
         <v>10</v>
       </c>
       <c r="I12">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J12" t="s">
         <v>18</v>
@@ -1112,39 +1112,39 @@
         <v>29</v>
       </c>
       <c r="L12">
-        <v>0.9249998331069946</v>
+        <v>0.9180000424385071</v>
       </c>
       <c r="M12">
-        <v>0.921999990940094</v>
+        <v>0.9309999942779541</v>
       </c>
       <c r="N12">
-        <v>0.9234999120235443</v>
+        <v>0.9245000183582306</v>
       </c>
       <c r="O12">
-        <v>0.001499921083450317</v>
+        <v>0.006499975919723511</v>
       </c>
       <c r="P12">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>111.5190763473511</v>
+        <v>125.7245346307755</v>
       </c>
       <c r="C13">
-        <v>1.212055206298828</v>
+        <v>0.02507269382476807</v>
       </c>
       <c r="D13">
-        <v>11.61174273490906</v>
+        <v>11.07002782821655</v>
       </c>
       <c r="E13">
-        <v>0.08298683166503906</v>
+        <v>0.3772299289703369</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G13">
         <v>25</v>
@@ -1156,22 +1156,22 @@
         <v>256</v>
       </c>
       <c r="J13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" t="s">
         <v>30</v>
       </c>
       <c r="L13">
-        <v>0.9319999814033508</v>
+        <v>0.9179998636245728</v>
       </c>
       <c r="M13">
-        <v>0.9140000343322754</v>
+        <v>0.9300000071525574</v>
       </c>
       <c r="N13">
-        <v>0.9230000078678131</v>
+        <v>0.9239999353885651</v>
       </c>
       <c r="O13">
-        <v>0.00899997353553772</v>
+        <v>0.00600007176399231</v>
       </c>
       <c r="P13">
         <v>12</v>
@@ -1179,31 +1179,31 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>115.1637585163116</v>
+        <v>126.364465713501</v>
       </c>
       <c r="C14">
-        <v>3.874695301055908</v>
+        <v>1.004800081253052</v>
       </c>
       <c r="D14">
-        <v>10.71052861213684</v>
+        <v>14.47601079940796</v>
       </c>
       <c r="E14">
-        <v>0.4466373920440674</v>
+        <v>0.4491820335388184</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G14">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J14" t="s">
         <v>17</v>
@@ -1212,16 +1212,16 @@
         <v>31</v>
       </c>
       <c r="L14">
-        <v>0.9230000376701355</v>
+        <v>0.9159998893737793</v>
       </c>
       <c r="M14">
-        <v>0.9209998846054077</v>
+        <v>0.9290000200271606</v>
       </c>
       <c r="N14">
-        <v>0.9219999611377716</v>
+        <v>0.92249995470047</v>
       </c>
       <c r="O14">
-        <v>0.001000076532363892</v>
+        <v>0.006500065326690674</v>
       </c>
       <c r="P14">
         <v>13</v>
@@ -1229,31 +1229,31 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B15">
-        <v>68.54301083087921</v>
+        <v>129.9487674236298</v>
       </c>
       <c r="C15">
-        <v>8.528471350669861</v>
+        <v>0.5719282627105713</v>
       </c>
       <c r="D15">
-        <v>11.91691446304321</v>
+        <v>16.08725142478943</v>
       </c>
       <c r="E15">
-        <v>0.7704586982727051</v>
+        <v>0.7139945030212402</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H15">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I15">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J15" t="s">
         <v>18</v>
@@ -1262,16 +1262,16 @@
         <v>32</v>
       </c>
       <c r="L15">
-        <v>0.9240000247955322</v>
+        <v>0.9079999327659607</v>
       </c>
       <c r="M15">
-        <v>0.9189999103546143</v>
+        <v>0.9300000071525574</v>
       </c>
       <c r="N15">
-        <v>0.9214999675750732</v>
+        <v>0.918999969959259</v>
       </c>
       <c r="O15">
-        <v>0.002500057220458984</v>
+        <v>0.01100003719329834</v>
       </c>
       <c r="P15">
         <v>14</v>
@@ -1279,49 +1279,49 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="1">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>142.9282509088516</v>
+        <v>119.8473525047302</v>
       </c>
       <c r="C16">
-        <v>0.9941028356552124</v>
+        <v>5.066308736801147</v>
       </c>
       <c r="D16">
-        <v>15.41558229923248</v>
+        <v>17.31737506389618</v>
       </c>
       <c r="E16">
-        <v>2.586351752281189</v>
+        <v>3.872718691825867</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
       </c>
       <c r="G16">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K16" t="s">
         <v>33</v>
       </c>
       <c r="L16">
-        <v>0.906999945640564</v>
+        <v>0.9049999713897705</v>
       </c>
       <c r="M16">
-        <v>0.9330000281333923</v>
+        <v>0.9300000071525574</v>
       </c>
       <c r="N16">
-        <v>0.9199999868869781</v>
+        <v>0.9174999892711639</v>
       </c>
       <c r="O16">
-        <v>0.01300004124641418</v>
+        <v>0.01250001788139343</v>
       </c>
       <c r="P16">
         <v>15</v>
@@ -1329,28 +1329,28 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="1">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B17">
-        <v>70.08843576908112</v>
+        <v>118.4926937818527</v>
       </c>
       <c r="C17">
-        <v>3.660466074943542</v>
+        <v>3.567718863487244</v>
       </c>
       <c r="D17">
-        <v>14.51486754417419</v>
+        <v>15.45566082000732</v>
       </c>
       <c r="E17">
-        <v>2.431852102279663</v>
+        <v>1.126487016677856</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
       </c>
       <c r="G17">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I17">
         <v>128</v>
@@ -1362,16 +1362,16 @@
         <v>34</v>
       </c>
       <c r="L17">
-        <v>0.9169999957084656</v>
+        <v>0.9240000247955322</v>
       </c>
       <c r="M17">
-        <v>0.9150000214576721</v>
+        <v>0.9059999585151672</v>
       </c>
       <c r="N17">
-        <v>0.9160000085830688</v>
+        <v>0.9149999916553497</v>
       </c>
       <c r="O17">
-        <v>0.0009999871253967285</v>
+        <v>0.009000033140182495</v>
       </c>
       <c r="P17">
         <v>16</v>
@@ -1379,31 +1379,31 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="1">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B18">
-        <v>85.05287992954254</v>
+        <v>57.47126758098602</v>
       </c>
       <c r="C18">
-        <v>8.842670083045959</v>
+        <v>5.525586009025574</v>
       </c>
       <c r="D18">
-        <v>17.13321840763092</v>
+        <v>11.08387088775635</v>
       </c>
       <c r="E18">
-        <v>2.617046713829041</v>
+        <v>0.9228942394256592</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
       </c>
       <c r="G18">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H18">
         <v>5</v>
       </c>
       <c r="I18">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J18" t="s">
         <v>18</v>
@@ -1412,16 +1412,16 @@
         <v>35</v>
       </c>
       <c r="L18">
-        <v>0.9319999814033508</v>
+        <v>0.9200000166893005</v>
       </c>
       <c r="M18">
-        <v>0.8989999890327454</v>
+        <v>0.8990001082420349</v>
       </c>
       <c r="N18">
-        <v>0.9154999852180481</v>
+        <v>0.9095000624656677</v>
       </c>
       <c r="O18">
-        <v>0.01649999618530273</v>
+        <v>0.01049995422363281</v>
       </c>
       <c r="P18">
         <v>17</v>
@@ -1432,19 +1432,19 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <v>86.62878847122192</v>
+        <v>68.2429758310318</v>
       </c>
       <c r="C19">
-        <v>13.71841716766357</v>
+        <v>7.858142018318176</v>
       </c>
       <c r="D19">
-        <v>14.19310760498047</v>
+        <v>12.56981289386749</v>
       </c>
       <c r="E19">
-        <v>2.428851366043091</v>
+        <v>1.35773766040802</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>20</v>
@@ -1462,16 +1462,16 @@
         <v>36</v>
       </c>
       <c r="L19">
-        <v>0.9160000085830688</v>
+        <v>0.9059999585151672</v>
       </c>
       <c r="M19">
         <v>0.9110000729560852</v>
       </c>
       <c r="N19">
-        <v>0.913500040769577</v>
+        <v>0.9085000157356262</v>
       </c>
       <c r="O19">
-        <v>0.002499967813491821</v>
+        <v>0.002500057220458984</v>
       </c>
       <c r="P19">
         <v>18</v>
@@ -1479,25 +1479,25 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="1">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>103.2003771066666</v>
+        <v>69.55311787128448</v>
       </c>
       <c r="C20">
-        <v>3.280528664588928</v>
+        <v>0.4260545969009399</v>
       </c>
       <c r="D20">
-        <v>12.4791522026062</v>
+        <v>15.99222481250763</v>
       </c>
       <c r="E20">
-        <v>0.8874263763427734</v>
+        <v>5.185613512992859</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H20">
         <v>5</v>
@@ -1506,22 +1506,22 @@
         <v>256</v>
       </c>
       <c r="J20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K20" t="s">
         <v>37</v>
       </c>
       <c r="L20">
-        <v>0.9210000038146973</v>
+        <v>0.9290000796318054</v>
       </c>
       <c r="M20">
-        <v>0.9049999713897705</v>
+        <v>0.8859999775886536</v>
       </c>
       <c r="N20">
-        <v>0.9129999876022339</v>
+        <v>0.9075000286102295</v>
       </c>
       <c r="O20">
-        <v>0.008000016212463379</v>
+        <v>0.02150005102157593</v>
       </c>
       <c r="P20">
         <v>19</v>
@@ -1529,25 +1529,25 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>112.3674980401993</v>
+        <v>65.49445104598999</v>
       </c>
       <c r="C21">
-        <v>1.912895798683167</v>
+        <v>10.41224074363708</v>
       </c>
       <c r="D21">
-        <v>13.88630616664886</v>
+        <v>11.31824338436127</v>
       </c>
       <c r="E21">
-        <v>0.4235292673110962</v>
+        <v>0.4063478708267212</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H21">
         <v>5</v>
@@ -1556,22 +1556,22 @@
         <v>128</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K21" t="s">
         <v>38</v>
       </c>
       <c r="L21">
-        <v>0.9079999327659607</v>
+        <v>0.8899999260902405</v>
       </c>
       <c r="M21">
-        <v>0.9169999957084656</v>
+        <v>0.925000011920929</v>
       </c>
       <c r="N21">
-        <v>0.9124999642372131</v>
+        <v>0.9074999690055847</v>
       </c>
       <c r="O21">
-        <v>0.004500031471252441</v>
+        <v>0.01750004291534424</v>
       </c>
       <c r="P21">
         <v>20</v>
@@ -1579,19 +1579,19 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="1">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>110.3258522748947</v>
+        <v>68.08357620239258</v>
       </c>
       <c r="C22">
-        <v>0.8902684450149536</v>
+        <v>11.72409248352051</v>
       </c>
       <c r="D22">
-        <v>11.02676975727081</v>
+        <v>12.07488679885864</v>
       </c>
       <c r="E22">
-        <v>0.1997205018997192</v>
+        <v>1.100916147232056</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
@@ -1600,28 +1600,28 @@
         <v>25</v>
       </c>
       <c r="H22">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I22">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K22" t="s">
         <v>39</v>
       </c>
       <c r="L22">
-        <v>0.906999945640564</v>
+        <v>0.9109998941421509</v>
       </c>
       <c r="M22">
-        <v>0.9139999151229858</v>
+        <v>0.8989999294281006</v>
       </c>
       <c r="N22">
-        <v>0.9104999303817749</v>
+        <v>0.9049999117851257</v>
       </c>
       <c r="O22">
-        <v>0.003499984741210938</v>
+        <v>0.005999982357025146</v>
       </c>
       <c r="P22">
         <v>21</v>
@@ -1629,25 +1629,25 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="1">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B23">
-        <v>81.08935630321503</v>
+        <v>67.88970410823822</v>
       </c>
       <c r="C23">
-        <v>18.50767362117767</v>
+        <v>13.40917956829071</v>
       </c>
       <c r="D23">
-        <v>19.50814354419708</v>
+        <v>11.90208196640015</v>
       </c>
       <c r="E23">
-        <v>5.129084944725037</v>
+        <v>0.4699547290802002</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H23">
         <v>5</v>
@@ -1656,22 +1656,22 @@
         <v>128</v>
       </c>
       <c r="J23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K23" t="s">
         <v>40</v>
       </c>
       <c r="L23">
-        <v>0.9049999117851257</v>
+        <v>0.9100000858306885</v>
       </c>
       <c r="M23">
-        <v>0.8939999341964722</v>
+        <v>0.8930000066757202</v>
       </c>
       <c r="N23">
-        <v>0.899499922990799</v>
+        <v>0.9015000462532043</v>
       </c>
       <c r="O23">
-        <v>0.005499988794326782</v>
+        <v>0.008500039577484131</v>
       </c>
       <c r="P23">
         <v>22</v>
@@ -1679,22 +1679,22 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="1">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B24">
-        <v>98.84335350990295</v>
+        <v>69.01125752925873</v>
       </c>
       <c r="C24">
-        <v>6.773154020309448</v>
+        <v>7.028479695320129</v>
       </c>
       <c r="D24">
-        <v>22.12243497371674</v>
+        <v>14.49444997310638</v>
       </c>
       <c r="E24">
-        <v>7.694762587547302</v>
+        <v>3.193894982337952</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24">
         <v>25</v>
@@ -1703,25 +1703,25 @@
         <v>5</v>
       </c>
       <c r="I24">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K24" t="s">
         <v>41</v>
       </c>
       <c r="L24">
-        <v>0.9129999279975891</v>
+        <v>0.8920000195503235</v>
       </c>
       <c r="M24">
-        <v>0.8819999098777771</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N24">
-        <v>0.8974999189376831</v>
+        <v>0.8959999978542328</v>
       </c>
       <c r="O24">
-        <v>0.01550000905990601</v>
+        <v>0.003999978303909302</v>
       </c>
       <c r="P24">
         <v>23</v>
@@ -1732,19 +1732,19 @@
         <v>12</v>
       </c>
       <c r="B25">
-        <v>112.8342931270599</v>
+        <v>121.3500519990921</v>
       </c>
       <c r="C25">
-        <v>6.430818557739258</v>
+        <v>1.071845412254333</v>
       </c>
       <c r="D25">
-        <v>771.8749134540558</v>
+        <v>19.80461192131042</v>
       </c>
       <c r="E25">
-        <v>761.3899502754211</v>
+        <v>2.736958026885986</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G25">
         <v>20</v>
@@ -1762,16 +1762,16 @@
         <v>42</v>
       </c>
       <c r="L25">
-        <v>0.8490000367164612</v>
+        <v>0.8610000610351562</v>
       </c>
       <c r="M25">
-        <v>0.937000036239624</v>
+        <v>0.9289999604225159</v>
       </c>
       <c r="N25">
-        <v>0.8930000364780426</v>
+        <v>0.8950000107288361</v>
       </c>
       <c r="O25">
-        <v>0.04399999976158142</v>
+        <v>0.03399994969367981</v>
       </c>
       <c r="P25">
         <v>24</v>
@@ -1779,31 +1779,31 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B26">
-        <v>56.08218157291412</v>
+        <v>130.9948101043701</v>
       </c>
       <c r="C26">
-        <v>2.893380761146545</v>
+        <v>0.91379714012146</v>
       </c>
       <c r="D26">
-        <v>11.26058793067932</v>
+        <v>11.27039086818695</v>
       </c>
       <c r="E26">
-        <v>0.9836664199829102</v>
+        <v>0.5099669694900513</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G26">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H26">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I26">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J26" t="s">
         <v>17</v>
@@ -1812,16 +1812,16 @@
         <v>43</v>
       </c>
       <c r="L26">
-        <v>0.8859999775886536</v>
+        <v>0.9019999504089355</v>
       </c>
       <c r="M26">
-        <v>0.8819999694824219</v>
+        <v>0.8869999647140503</v>
       </c>
       <c r="N26">
-        <v>0.8839999735355377</v>
+        <v>0.8944999575614929</v>
       </c>
       <c r="O26">
-        <v>0.002000004053115845</v>
+        <v>0.007499992847442627</v>
       </c>
       <c r="P26">
         <v>25</v>
@@ -1829,22 +1829,22 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B27">
-        <v>58.81357645988464</v>
+        <v>62.17344617843628</v>
       </c>
       <c r="C27">
-        <v>3.650204420089722</v>
+        <v>2.636117935180664</v>
       </c>
       <c r="D27">
-        <v>11.54615926742554</v>
+        <v>14.2640837430954</v>
       </c>
       <c r="E27">
-        <v>0.1006989479064941</v>
+        <v>3.563422799110413</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G27">
         <v>20</v>
@@ -1853,7 +1853,7 @@
         <v>5</v>
       </c>
       <c r="I27">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J27" t="s">
         <v>18</v>
@@ -1862,16 +1862,16 @@
         <v>44</v>
       </c>
       <c r="L27">
-        <v>0.8709999918937683</v>
+        <v>0.8759999871253967</v>
       </c>
       <c r="M27">
-        <v>0.8939999938011169</v>
+        <v>0.8829999566078186</v>
       </c>
       <c r="N27">
-        <v>0.8824999928474426</v>
+        <v>0.8794999718666077</v>
       </c>
       <c r="O27">
-        <v>0.01150000095367432</v>
+        <v>0.003499984741210938</v>
       </c>
       <c r="P27">
         <v>26</v>
@@ -1879,31 +1879,31 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B28">
-        <v>59.57585680484772</v>
+        <v>59.33847689628601</v>
       </c>
       <c r="C28">
-        <v>0.6418379545211792</v>
+        <v>6.576913595199585</v>
       </c>
       <c r="D28">
-        <v>11.83613276481628</v>
+        <v>11.78625881671906</v>
       </c>
       <c r="E28">
-        <v>1.074345111846924</v>
+        <v>1.240326762199402</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G28">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H28">
         <v>5</v>
       </c>
       <c r="I28">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J28" t="s">
         <v>17</v>
@@ -1912,16 +1912,16 @@
         <v>45</v>
       </c>
       <c r="L28">
-        <v>0.8960000872612</v>
+        <v>0.8980000019073486</v>
       </c>
       <c r="M28">
-        <v>0.8540000319480896</v>
+        <v>0.8600000143051147</v>
       </c>
       <c r="N28">
-        <v>0.8750000596046448</v>
+        <v>0.8790000081062317</v>
       </c>
       <c r="O28">
-        <v>0.02100002765655518</v>
+        <v>0.01899999380111694</v>
       </c>
       <c r="P28">
         <v>27</v>
@@ -1929,25 +1929,25 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B29">
-        <v>55.76097989082336</v>
+        <v>64.50617527961731</v>
       </c>
       <c r="C29">
-        <v>2.686948776245117</v>
+        <v>1.016768217086792</v>
       </c>
       <c r="D29">
-        <v>10.45479798316956</v>
+        <v>16.01243078708649</v>
       </c>
       <c r="E29">
-        <v>0.2495784759521484</v>
+        <v>5.405982375144958</v>
       </c>
       <c r="F29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G29">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H29">
         <v>5</v>
@@ -1962,16 +1962,16 @@
         <v>46</v>
       </c>
       <c r="L29">
-        <v>0.8919999599456787</v>
+        <v>0.9099999070167542</v>
       </c>
       <c r="M29">
-        <v>0.8510000705718994</v>
+        <v>0.8339999914169312</v>
       </c>
       <c r="N29">
-        <v>0.8715000152587891</v>
+        <v>0.8719999492168427</v>
       </c>
       <c r="O29">
-        <v>0.02049994468688965</v>
+        <v>0.0379999577999115</v>
       </c>
       <c r="P29">
         <v>28</v>
@@ -1979,22 +1979,22 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30">
-        <v>52.34040093421936</v>
+        <v>55.14483439922333</v>
       </c>
       <c r="C30">
-        <v>1.535679340362549</v>
+        <v>3.815409779548645</v>
       </c>
       <c r="D30">
-        <v>10.10178458690643</v>
+        <v>10.18251729011536</v>
       </c>
       <c r="E30">
-        <v>0.07559406757354736</v>
+        <v>0.002393245697021484</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G30">
         <v>25</v>
@@ -2006,22 +2006,22 @@
         <v>256</v>
       </c>
       <c r="J30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K30" t="s">
         <v>47</v>
       </c>
       <c r="L30">
-        <v>0.8380000591278076</v>
+        <v>0.8439999222755432</v>
       </c>
       <c r="M30">
-        <v>0.8940001130104065</v>
+        <v>0.8579999804496765</v>
       </c>
       <c r="N30">
-        <v>0.8660000860691071</v>
+        <v>0.8509999513626099</v>
       </c>
       <c r="O30">
-        <v>0.02800002694129944</v>
+        <v>0.00700002908706665</v>
       </c>
       <c r="P30">
         <v>29</v>
@@ -2029,22 +2029,22 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B31">
-        <v>59.78808236122131</v>
+        <v>64.04184758663177</v>
       </c>
       <c r="C31">
-        <v>2.484103918075562</v>
+        <v>5.550500273704529</v>
       </c>
       <c r="D31">
-        <v>12.01153135299683</v>
+        <v>13.28271973133087</v>
       </c>
       <c r="E31">
-        <v>1.047560214996338</v>
+        <v>2.686355948448181</v>
       </c>
       <c r="F31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G31">
         <v>20</v>
@@ -2053,25 +2053,25 @@
         <v>5</v>
       </c>
       <c r="I31">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K31" t="s">
         <v>48</v>
       </c>
       <c r="L31">
-        <v>0.8409999012947083</v>
+        <v>0.7880000472068787</v>
       </c>
       <c r="M31">
-        <v>0.887999951839447</v>
+        <v>0.9079999327659607</v>
       </c>
       <c r="N31">
-        <v>0.8644999265670776</v>
+        <v>0.8479999899864197</v>
       </c>
       <c r="O31">
-        <v>0.02350002527236938</v>
+        <v>0.05999994277954102</v>
       </c>
       <c r="P31">
         <v>30</v>
@@ -2079,22 +2079,22 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32">
-        <v>56.04004621505737</v>
+        <v>63.9830105304718</v>
       </c>
       <c r="C32">
-        <v>0.2442131042480469</v>
+        <v>4.111819267272949</v>
       </c>
       <c r="D32">
-        <v>12.55375599861145</v>
+        <v>14.20074081420898</v>
       </c>
       <c r="E32">
-        <v>0.0222628116607666</v>
+        <v>3.569218635559082</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G32">
         <v>20</v>
@@ -2103,25 +2103,25 @@
         <v>5</v>
       </c>
       <c r="I32">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K32" t="s">
         <v>49</v>
       </c>
       <c r="L32">
-        <v>0.8349999189376831</v>
+        <v>0.8320000171661377</v>
       </c>
       <c r="M32">
-        <v>0.8680000305175781</v>
+        <v>0.8579999804496765</v>
       </c>
       <c r="N32">
-        <v>0.8514999747276306</v>
+        <v>0.8449999988079071</v>
       </c>
       <c r="O32">
-        <v>0.01650005578994751</v>
+        <v>0.01299998164176941</v>
       </c>
       <c r="P32">
         <v>31</v>
@@ -2129,22 +2129,22 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B33">
-        <v>55.50199258327484</v>
+        <v>50.55229723453522</v>
       </c>
       <c r="C33">
-        <v>2.926184773445129</v>
+        <v>0.5196291208267212</v>
       </c>
       <c r="D33">
-        <v>10.69364142417908</v>
+        <v>10.05489933490753</v>
       </c>
       <c r="E33">
-        <v>0.212160587310791</v>
+        <v>0.01196372509002686</v>
       </c>
       <c r="F33" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G33">
         <v>25</v>
@@ -2153,7 +2153,7 @@
         <v>5</v>
       </c>
       <c r="I33">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J33" t="s">
         <v>18</v>
@@ -2162,16 +2162,16 @@
         <v>50</v>
       </c>
       <c r="L33">
+        <v>0.7769999504089355</v>
+      </c>
+      <c r="M33">
+        <v>0.875</v>
+      </c>
+      <c r="N33">
         <v>0.8259999752044678</v>
       </c>
-      <c r="M33">
-        <v>0.8690000176429749</v>
-      </c>
-      <c r="N33">
-        <v>0.8474999964237213</v>
-      </c>
       <c r="O33">
-        <v>0.02150002121925354</v>
+        <v>0.04900002479553223</v>
       </c>
       <c r="P33">
         <v>32</v>

</xml_diff>